<commit_message>
Fixed state social benefits add factor
</commit_message>
<xml_diff>
--- a/comparison.xlsx
+++ b/comparison.xlsx
@@ -1285,7 +1285,7 @@
         <v>68.930270815822</v>
       </c>
       <c r="E6" t="n">
-        <v>68.930270815822</v>
+        <v>67.261751256205</v>
       </c>
     </row>
     <row r="7">
@@ -1302,7 +1302,7 @@
         <v>64.768464790714</v>
       </c>
       <c r="E7" t="n">
-        <v>64.768464790714</v>
+        <v>63.106744514583</v>
       </c>
     </row>
     <row r="8">
@@ -1319,7 +1319,7 @@
         <v>62.2254499609565</v>
       </c>
       <c r="E8" t="n">
-        <v>62.2254499609565</v>
+        <v>60.5484628120389</v>
       </c>
     </row>
     <row r="9">
@@ -1336,7 +1336,7 @@
         <v>50.450612536016</v>
       </c>
       <c r="E9" t="n">
-        <v>50.450612536016</v>
+        <v>48.7568262098614</v>
       </c>
     </row>
     <row r="10">
@@ -1353,7 +1353,7 @@
         <v>48.7850626383487</v>
       </c>
       <c r="E10" t="n">
-        <v>48.7850626383487</v>
+        <v>47.075168778348</v>
       </c>
     </row>
     <row r="11">
@@ -1370,7 +1370,7 @@
         <v>47.1083813115638</v>
       </c>
       <c r="E11" t="n">
-        <v>47.1083813115638</v>
+        <v>45.3822863482939</v>
       </c>
     </row>
     <row r="12">
@@ -1387,7 +1387,7 @@
         <v>45.3772834732095</v>
       </c>
       <c r="E12" t="n">
-        <v>45.3772834732095</v>
+        <v>43.6346115354096</v>
       </c>
     </row>
     <row r="13">
@@ -1404,7 +1404,7 @@
         <v>43.6489440258087</v>
       </c>
       <c r="E13" t="n">
-        <v>43.6489440258087</v>
+        <v>41.889691937128</v>
       </c>
     </row>
     <row r="14">
@@ -1489,7 +1489,7 @@
         <v>21.9001687008999</v>
       </c>
       <c r="E18" t="n">
-        <v>21.9001687008999</v>
+        <v>27.2402301758955</v>
       </c>
     </row>
     <row r="19">
@@ -1506,7 +1506,7 @@
         <v>53.5804168398504</v>
       </c>
       <c r="E19" t="n">
-        <v>53.5804168398504</v>
+        <v>58.9204783148459</v>
       </c>
     </row>
     <row r="20">
@@ -1523,7 +1523,7 @@
         <v>54.7490971757863</v>
       </c>
       <c r="E20" t="n">
-        <v>54.7490971757863</v>
+        <v>60.2056345053309</v>
       </c>
     </row>
     <row r="21">
@@ -1540,7 +1540,7 @@
         <v>55.9177775117221</v>
       </c>
       <c r="E21" t="n">
-        <v>55.9177775117221</v>
+        <v>61.4907906958156</v>
       </c>
     </row>
     <row r="22">
@@ -1557,7 +1557,7 @@
         <v>57.0864578476576</v>
       </c>
       <c r="E22" t="n">
-        <v>57.0864578476576</v>
+        <v>62.7759468863001</v>
       </c>
     </row>
     <row r="23">
@@ -1574,7 +1574,7 @@
         <v>58.2551381835935</v>
       </c>
       <c r="E23" t="n">
-        <v>58.2551381835935</v>
+        <v>64.0611030767852</v>
       </c>
     </row>
     <row r="24">
@@ -1591,7 +1591,7 @@
         <v>58.7506778104657</v>
       </c>
       <c r="E24" t="n">
-        <v>58.7506778104657</v>
+        <v>64.6060303759987</v>
       </c>
     </row>
     <row r="25">
@@ -1608,7 +1608,7 @@
         <v>59.2462174373377</v>
       </c>
       <c r="E25" t="n">
-        <v>59.2462174373377</v>
+        <v>65.1509576752117</v>
       </c>
     </row>
     <row r="26">
@@ -1897,7 +1897,7 @@
         <v>245.49251687692</v>
       </c>
       <c r="E42" t="n">
-        <v>245.49251687692</v>
+        <v>292.56851838171</v>
       </c>
     </row>
     <row r="43">
@@ -1914,7 +1914,7 @@
         <v>184.802218709821</v>
       </c>
       <c r="E43" t="n">
-        <v>184.802218709821</v>
+        <v>231.349925463324</v>
       </c>
     </row>
     <row r="44">
@@ -1931,7 +1931,7 @@
         <v>168.771574790086</v>
       </c>
       <c r="E44" t="n">
-        <v>168.771574790086</v>
+        <v>216.025400379625</v>
       </c>
     </row>
     <row r="45">
@@ -1948,7 +1948,7 @@
         <v>168.921154689145</v>
       </c>
       <c r="E45" t="n">
-        <v>168.921154689145</v>
+        <v>216.211577832086</v>
       </c>
     </row>
     <row r="46">
@@ -1965,7 +1965,7 @@
         <v>168.287137334798</v>
       </c>
       <c r="E46" t="n">
-        <v>168.287137334798</v>
+        <v>215.393992553534</v>
       </c>
     </row>
     <row r="47">
@@ -1982,7 +1982,7 @@
         <v>166.480628169955</v>
       </c>
       <c r="E47" t="n">
-        <v>166.480628169955</v>
+        <v>213.074483197684</v>
       </c>
     </row>
     <row r="48">
@@ -1999,7 +1999,7 @@
         <v>168.625348242122</v>
       </c>
       <c r="E48" t="n">
-        <v>168.625348242122</v>
+        <v>215.818191687277</v>
       </c>
     </row>
     <row r="49">
@@ -2016,7 +2016,7 @@
         <v>169.743569380959</v>
       </c>
       <c r="E49" t="n">
-        <v>169.743569380959</v>
+        <v>217.246988252124</v>
       </c>
     </row>
     <row r="50">
@@ -2101,7 +2101,7 @@
         <v>443.198201747099</v>
       </c>
       <c r="E54" t="n">
-        <v>443.198201747099</v>
+        <v>442.796327144478</v>
       </c>
     </row>
     <row r="55">
@@ -2118,7 +2118,7 @@
         <v>-298.697164901108</v>
       </c>
       <c r="E55" t="n">
-        <v>-298.697164901108</v>
+        <v>-299.100957177089</v>
       </c>
     </row>
     <row r="56">
@@ -2135,7 +2135,7 @@
         <v>-305.331724383166</v>
       </c>
       <c r="E56" t="n">
-        <v>-305.331724383166</v>
+        <v>-305.73747330127</v>
       </c>
     </row>
     <row r="57">
@@ -2152,7 +2152,7 @@
         <v>-332.742307786574</v>
       </c>
       <c r="E57" t="n">
-        <v>-332.742307786574</v>
+        <v>-333.150035907665</v>
       </c>
     </row>
     <row r="58">
@@ -2169,7 +2169,7 @@
         <v>-334.347470230323</v>
       </c>
       <c r="E58" t="n">
-        <v>-334.347470230323</v>
+        <v>-334.757165248474</v>
       </c>
     </row>
     <row r="59">
@@ -2186,7 +2186,7 @@
         <v>-335.927525857953</v>
       </c>
       <c r="E59" t="n">
-        <v>-335.927525857953</v>
+        <v>-336.339157008352</v>
       </c>
     </row>
     <row r="60">
@@ -2203,7 +2203,7 @@
         <v>-337.497538759138</v>
       </c>
       <c r="E60" t="n">
-        <v>-337.497538759138</v>
+        <v>-337.911093735859</v>
       </c>
     </row>
     <row r="61">
@@ -2220,7 +2220,7 @@
         <v>-339.064204084839</v>
       </c>
       <c r="E61" t="n">
-        <v>-339.064204084839</v>
+        <v>-339.479678785908</v>
       </c>
     </row>
     <row r="62">
@@ -2509,7 +2509,7 @@
         <v>-1.97661859993192</v>
       </c>
       <c r="E78" t="n">
-        <v>-1.97661859993192</v>
+        <v>-2.63171170731439</v>
       </c>
     </row>
     <row r="79">
@@ -2526,7 +2526,7 @@
         <v>-2.00523604800819</v>
       </c>
       <c r="E79" t="n">
-        <v>-2.00523604800819</v>
+        <v>-2.66981358146363</v>
       </c>
     </row>
     <row r="80">
@@ -2543,7 +2543,7 @@
         <v>-2.0318925382844</v>
       </c>
       <c r="E80" t="n">
-        <v>-2.0318925382844</v>
+        <v>-2.70530459502497</v>
       </c>
     </row>
     <row r="81">
@@ -2713,7 +2713,7 @@
         <v>12.1910004759371</v>
       </c>
       <c r="E90" t="n">
-        <v>12.1910004759371</v>
+        <v>6.78788008576706</v>
       </c>
     </row>
     <row r="91">
@@ -2730,7 +2730,7 @@
         <v>8.0446176857161</v>
       </c>
       <c r="E91" t="n">
-        <v>8.0446176857161</v>
+        <v>2.46213908983606</v>
       </c>
     </row>
     <row r="92">
@@ -2747,7 +2747,7 @@
         <v>7.4595249346371</v>
       </c>
       <c r="E92" t="n">
-        <v>7.4595249346371</v>
+        <v>1.85173724615305</v>
       </c>
     </row>
     <row r="93">
@@ -2764,7 +2764,7 @@
         <v>6.8744321835571</v>
       </c>
       <c r="E93" t="n">
-        <v>6.8744321835571</v>
+        <v>1.24133540247004</v>
       </c>
     </row>
     <row r="94">
@@ -2781,7 +2781,7 @@
         <v>47.9372740323607</v>
       </c>
       <c r="E94" t="n">
-        <v>47.9372740323607</v>
+        <v>42.7118461161017</v>
       </c>
     </row>
     <row r="95">
@@ -2798,7 +2798,7 @@
         <v>47.3521812812807</v>
       </c>
       <c r="E95" t="n">
-        <v>47.3521812812807</v>
+        <v>42.1014442724187</v>
       </c>
     </row>
     <row r="96">
@@ -2815,7 +2815,7 @@
         <v>49.2452983787097</v>
       </c>
       <c r="E96" t="n">
-        <v>49.2452983787097</v>
+        <v>44.0764510802217</v>
       </c>
     </row>
     <row r="97">
@@ -2832,7 +2832,7 @@
         <v>48.7060299634791</v>
       </c>
       <c r="E97" t="n">
-        <v>48.7060299634791</v>
+        <v>43.5937849434418</v>
       </c>
     </row>
     <row r="98">
@@ -2917,7 +2917,7 @@
         <v>-27.5404605256526</v>
       </c>
       <c r="E102" t="n">
-        <v>-27.5404605256526</v>
+        <v>-27.7374595279825</v>
       </c>
     </row>
     <row r="103">
@@ -2934,7 +2934,7 @@
         <v>-27.9391908113569</v>
       </c>
       <c r="E103" t="n">
-        <v>-27.9391908113569</v>
+        <v>-28.139041961663</v>
       </c>
     </row>
     <row r="104">
@@ -2951,7 +2951,7 @@
         <v>-28.3105988403252</v>
       </c>
       <c r="E104" t="n">
-        <v>-28.3105988403252</v>
+        <v>-28.5131067004138</v>
       </c>
     </row>
     <row r="105">
@@ -3325,7 +3325,7 @@
         <v>41.2053007972779</v>
       </c>
       <c r="E126" t="n">
-        <v>41.2053007972779</v>
+        <v>41.2546570673381</v>
       </c>
     </row>
     <row r="127">
@@ -3342,7 +3342,7 @@
         <v>42.7203446507589</v>
       </c>
       <c r="E127" t="n">
-        <v>42.7203446507589</v>
+        <v>42.8080107045492</v>
       </c>
     </row>
     <row r="128">
@@ -3359,7 +3359,7 @@
         <v>32.4662493820931</v>
       </c>
       <c r="E128" t="n">
-        <v>32.4662493820931</v>
+        <v>32.4619120592484</v>
       </c>
     </row>
     <row r="129">
@@ -3376,7 +3376,7 @@
         <v>22.3705205143364</v>
       </c>
       <c r="E129" t="n">
-        <v>22.3705205143364</v>
+        <v>22.2724199727681</v>
       </c>
     </row>
     <row r="130">
@@ -3393,7 +3393,7 @@
         <v>23.9156335401083</v>
       </c>
       <c r="E130" t="n">
-        <v>23.9156335401083</v>
+        <v>23.8220154247228</v>
       </c>
     </row>
     <row r="131">
@@ -3410,7 +3410,7 @@
         <v>25.3476666731361</v>
       </c>
       <c r="E131" t="n">
-        <v>25.3476666731361</v>
+        <v>25.2581606674566</v>
       </c>
     </row>
     <row r="132">
@@ -3427,7 +3427,7 @@
         <v>28.0195179962026</v>
       </c>
       <c r="E132" t="n">
-        <v>28.0195179962026</v>
+        <v>27.9406305173514</v>
       </c>
     </row>
     <row r="133">
@@ -3444,7 +3444,7 @@
         <v>30.565599506059</v>
       </c>
       <c r="E133" t="n">
-        <v>30.565599506059</v>
+        <v>30.4969186803337</v>
       </c>
     </row>
     <row r="134">
@@ -4515,7 +4515,7 @@
         <v>294.151</v>
       </c>
       <c r="E196" t="n">
-        <v>294.151</v>
+        <v>294.149</v>
       </c>
     </row>
     <row r="197">
@@ -4532,7 +4532,7 @@
         <v>322.638804</v>
       </c>
       <c r="E197" t="n">
-        <v>322.638804</v>
+        <v>322.636796</v>
       </c>
     </row>
     <row r="198">
@@ -4549,7 +4549,7 @@
         <v>324.529759216</v>
       </c>
       <c r="E198" t="n">
-        <v>324.529759216</v>
+        <v>324.527743184</v>
       </c>
     </row>
     <row r="199">
@@ -4566,7 +4566,7 @@
         <v>319.323878252864</v>
       </c>
       <c r="E199" t="n">
-        <v>319.323878252864</v>
+        <v>319.321854156736</v>
       </c>
     </row>
     <row r="200">
@@ -4583,7 +4583,7 @@
         <v>319.121173765875</v>
       </c>
       <c r="E200" t="n">
-        <v>319.121173765875</v>
+        <v>319.119141573363</v>
       </c>
     </row>
     <row r="201">
@@ -4600,7 +4600,7 @@
         <v>309.921658460939</v>
       </c>
       <c r="E201" t="n">
-        <v>309.921658460939</v>
+        <v>309.919618139656</v>
       </c>
     </row>
     <row r="202">
@@ -4617,7 +4617,7 @@
         <v>310.725345094783</v>
       </c>
       <c r="E202" t="n">
-        <v>310.725345094783</v>
+        <v>310.723296612215</v>
       </c>
     </row>
     <row r="203">
@@ -4634,7 +4634,7 @@
         <v>311.532246475162</v>
       </c>
       <c r="E203" t="n">
-        <v>311.532246475162</v>
+        <v>311.530189798664</v>
       </c>
     </row>
     <row r="204">
@@ -4651,7 +4651,7 @@
         <v>312.342375461062</v>
       </c>
       <c r="E204" t="n">
-        <v>312.342375461062</v>
+        <v>312.340310557859</v>
       </c>
     </row>
     <row r="205">
@@ -4668,7 +4668,7 @@
         <v>313.155744962907</v>
       </c>
       <c r="E205" t="n">
-        <v>313.155744962907</v>
+        <v>313.15367180009</v>
       </c>
     </row>
     <row r="206">
@@ -4923,7 +4923,7 @@
         <v>-0.0181693268594994</v>
       </c>
       <c r="E220" t="n">
-        <v>-0.0181693268594994</v>
+        <v>-0.0182071156485106</v>
       </c>
     </row>
     <row r="221">
@@ -4940,7 +4940,7 @@
         <v>0.396371760332121</v>
       </c>
       <c r="E221" t="n">
-        <v>0.400047503566708</v>
+        <v>0.400048239196588</v>
       </c>
     </row>
     <row r="222">
@@ -4957,7 +4957,7 @@
         <v>-0.0367648043453786</v>
       </c>
       <c r="E222" t="n">
-        <v>-0.0367446396142885</v>
+        <v>-0.0367443431754113</v>
       </c>
     </row>
     <row r="223">
@@ -4974,7 +4974,7 @@
         <v>-0.159102764598621</v>
       </c>
       <c r="E223" t="n">
-        <v>-0.159015500038916</v>
+        <v>-0.159015237360191</v>
       </c>
     </row>
     <row r="224">
@@ -4991,7 +4991,7 @@
         <v>-0.06762001015531</v>
       </c>
       <c r="E224" t="n">
-        <v>-0.0675829219851056</v>
+        <v>-0.0675826595656327</v>
       </c>
     </row>
     <row r="225">
@@ -5008,7 +5008,7 @@
         <v>-0.22968130770882</v>
       </c>
       <c r="E225" t="n">
-        <v>-0.229555332285074</v>
+        <v>-0.229555035204657</v>
       </c>
     </row>
     <row r="226">
@@ -5025,7 +5025,7 @@
         <v>-0.0530986181339807</v>
       </c>
       <c r="E226" t="n">
-        <v>-0.0530694946454978</v>
+        <v>-0.0530691947703863</v>
       </c>
     </row>
     <row r="227">
@@ -5042,7 +5042,7 @@
         <v>-0.052904218192839</v>
       </c>
       <c r="E227" t="n">
-        <v>-0.0528752013286836</v>
+        <v>-0.0528749018168579</v>
       </c>
     </row>
     <row r="228">
@@ -5059,7 +5059,7 @@
         <v>-0.053062950596157</v>
       </c>
       <c r="E228" t="n">
-        <v>-0.0530338466705773</v>
+        <v>-0.0530335451691021</v>
       </c>
     </row>
     <row r="229">
@@ -5076,7 +5076,7 @@
         <v>-0.0521620068532343</v>
       </c>
       <c r="E229" t="n">
-        <v>-0.0521333970765731</v>
+        <v>-0.0521331006010142</v>
       </c>
     </row>
     <row r="230">
@@ -6147,7 +6147,7 @@
         <v>294.151</v>
       </c>
       <c r="E292" t="n">
-        <v>294.151</v>
+        <v>294.149</v>
       </c>
     </row>
     <row r="293">
@@ -6164,7 +6164,7 @@
         <v>322.638804</v>
       </c>
       <c r="E293" t="n">
-        <v>322.638804</v>
+        <v>322.636796</v>
       </c>
     </row>
     <row r="294">
@@ -6181,7 +6181,7 @@
         <v>324.529759216</v>
       </c>
       <c r="E294" t="n">
-        <v>324.529759216</v>
+        <v>324.527743184</v>
       </c>
     </row>
     <row r="295">
@@ -6198,7 +6198,7 @@
         <v>319.323878252864</v>
       </c>
       <c r="E295" t="n">
-        <v>319.323878252864</v>
+        <v>319.321854156736</v>
       </c>
     </row>
     <row r="296">
@@ -6215,7 +6215,7 @@
         <v>319.121173765875</v>
       </c>
       <c r="E296" t="n">
-        <v>319.121173765875</v>
+        <v>319.119141573363</v>
       </c>
     </row>
     <row r="297">
@@ -6232,7 +6232,7 @@
         <v>309.921658460939</v>
       </c>
       <c r="E297" t="n">
-        <v>309.921658460939</v>
+        <v>309.919618139656</v>
       </c>
     </row>
     <row r="298">
@@ -6249,7 +6249,7 @@
         <v>310.725345094783</v>
       </c>
       <c r="E298" t="n">
-        <v>310.725345094783</v>
+        <v>310.723296612215</v>
       </c>
     </row>
     <row r="299">
@@ -6266,7 +6266,7 @@
         <v>311.532246475162</v>
       </c>
       <c r="E299" t="n">
-        <v>311.532246475162</v>
+        <v>311.530189798664</v>
       </c>
     </row>
     <row r="300">
@@ -6283,7 +6283,7 @@
         <v>312.342375461062</v>
       </c>
       <c r="E300" t="n">
-        <v>312.342375461062</v>
+        <v>312.340310557859</v>
       </c>
     </row>
     <row r="301">
@@ -6300,7 +6300,7 @@
         <v>313.155744962907</v>
       </c>
       <c r="E301" t="n">
-        <v>313.155744962907</v>
+        <v>313.15367180009</v>
       </c>
     </row>
     <row r="302">
@@ -9411,7 +9411,7 @@
         <v>-0.222919776949612</v>
       </c>
       <c r="E484" t="n">
-        <v>-0.222919776949612</v>
+        <v>-0.222957565738623</v>
       </c>
     </row>
     <row r="485">
@@ -9428,7 +9428,7 @@
         <v>1.14845664155147</v>
       </c>
       <c r="E485" t="n">
-        <v>1.14617037148062</v>
+        <v>1.1461711071105</v>
       </c>
     </row>
     <row r="486">
@@ -9445,7 +9445,7 @@
         <v>0.549695710469531</v>
       </c>
       <c r="E486" t="n">
-        <v>0.549535119012968</v>
+        <v>0.549535415451845</v>
       </c>
     </row>
     <row r="487">
@@ -9462,7 +9462,7 @@
         <v>0.344162558280524</v>
       </c>
       <c r="E487" t="n">
-        <v>0.344042000695761</v>
+        <v>0.344042263374486</v>
       </c>
     </row>
     <row r="488">
@@ -9479,7 +9479,7 @@
         <v>0.0770714602230371</v>
       </c>
       <c r="E488" t="n">
-        <v>0.0770441554729193</v>
+        <v>0.0770444178923921</v>
       </c>
     </row>
     <row r="489">
@@ -9496,7 +9496,7 @@
         <v>-0.25079403615221</v>
       </c>
       <c r="E489" t="n">
-        <v>-0.25063890348388</v>
+        <v>-0.250638606403463</v>
       </c>
     </row>
     <row r="490">
@@ -9513,7 +9513,7 @@
         <v>0.0307363849571795</v>
       </c>
       <c r="E490" t="n">
-        <v>0.0307424886839985</v>
+        <v>0.03074278855911</v>
       </c>
     </row>
     <row r="491">
@@ -9530,7 +9530,7 @@
         <v>0.0966529345342258</v>
       </c>
       <c r="E491" t="n">
-        <v>0.0966220573993518</v>
+        <v>0.0966223569111774</v>
       </c>
     </row>
     <row r="492">
@@ -9547,7 +9547,7 @@
         <v>0.0931237076844637</v>
       </c>
       <c r="E492" t="n">
-        <v>0.0930947542130499</v>
+        <v>0.0930950557145251</v>
       </c>
     </row>
     <row r="493">
@@ -9564,7 +9564,7 @@
         <v>-0.0780924448983262</v>
       </c>
       <c r="E493" t="n">
-        <v>-0.0780276222839161</v>
+        <v>-0.0780273258083573</v>
       </c>
     </row>
     <row r="494">
@@ -11689,7 +11689,7 @@
         <v>1416.53969581915</v>
       </c>
       <c r="E618" t="n">
-        <v>1416.53969581915</v>
+        <v>1421.87975729415</v>
       </c>
     </row>
     <row r="619">
@@ -11706,7 +11706,7 @@
         <v>1439.59647107635</v>
       </c>
       <c r="E619" t="n">
-        <v>1439.59647107635</v>
+        <v>1444.93653255135</v>
       </c>
     </row>
     <row r="620">
@@ -11723,7 +11723,7 @@
         <v>1470.99652704191</v>
       </c>
       <c r="E620" t="n">
-        <v>1470.99652704191</v>
+        <v>1476.45306437146</v>
       </c>
     </row>
     <row r="621">
@@ -11740,7 +11740,7 @@
         <v>1502.39658300747</v>
       </c>
       <c r="E621" t="n">
-        <v>1502.39658300747</v>
+        <v>1507.96959619156</v>
       </c>
     </row>
     <row r="622">
@@ -11757,7 +11757,7 @@
         <v>1533.79663897303</v>
       </c>
       <c r="E622" t="n">
-        <v>1533.79663897303</v>
+        <v>1539.48612801167</v>
       </c>
     </row>
     <row r="623">
@@ -11774,7 +11774,7 @@
         <v>1565.19669493859</v>
       </c>
       <c r="E623" t="n">
-        <v>1565.19669493859</v>
+        <v>1571.00265983178</v>
       </c>
     </row>
     <row r="624">
@@ -11791,7 +11791,7 @@
         <v>1578.51083357726</v>
       </c>
       <c r="E624" t="n">
-        <v>1578.51083357726</v>
+        <v>1584.36618614279</v>
       </c>
     </row>
     <row r="625">
@@ -11808,7 +11808,7 @@
         <v>1591.82497221593</v>
       </c>
       <c r="E625" t="n">
-        <v>1591.82497221593</v>
+        <v>1597.72971245381</v>
       </c>
     </row>
     <row r="626">
@@ -12097,7 +12097,7 @@
         <v>0.0833726118806718</v>
       </c>
       <c r="E642" t="n">
-        <v>0.0805225308916535</v>
+        <v>0.10230783222657</v>
       </c>
     </row>
     <row r="643">
@@ -12114,7 +12114,7 @@
         <v>0.223738990224466</v>
       </c>
       <c r="E643" t="n">
-        <v>0.22084037772343</v>
+        <v>0.242190633030168</v>
       </c>
     </row>
     <row r="644">
@@ -12131,7 +12131,7 @@
         <v>0.16287026280409</v>
       </c>
       <c r="E644" t="n">
-        <v>0.160044651354156</v>
+        <v>0.181367029359166</v>
       </c>
     </row>
     <row r="645">
@@ -12148,7 +12148,7 @@
         <v>0.179470527467995</v>
       </c>
       <c r="E645" t="n">
-        <v>0.179372091613666</v>
+        <v>0.200662875487155</v>
       </c>
     </row>
     <row r="646">
@@ -12165,7 +12165,7 @@
         <v>0.241385729002343</v>
       </c>
       <c r="E646" t="n">
-        <v>0.241253333946773</v>
+        <v>0.241813088899492</v>
       </c>
     </row>
     <row r="647">
@@ -12182,7 +12182,7 @@
         <v>0.270250967377647</v>
       </c>
       <c r="E647" t="n">
-        <v>0.270102740338743</v>
+        <v>0.271104663632495</v>
       </c>
     </row>
     <row r="648">
@@ -12199,7 +12199,7 @@
         <v>0.190486411041974</v>
       </c>
       <c r="E648" t="n">
-        <v>0.19038193320445</v>
+        <v>0.191088138899913</v>
       </c>
     </row>
     <row r="649">
@@ -12216,7 +12216,7 @@
         <v>0.118970335385442</v>
       </c>
       <c r="E649" t="n">
-        <v>0.118905082629077</v>
+        <v>0.119346150986555</v>
       </c>
     </row>
     <row r="650">
@@ -12301,7 +12301,7 @@
         <v>0.884671409944758</v>
       </c>
       <c r="E654" t="n">
-        <v>0.884671409944758</v>
+        <v>6.22473288494029</v>
       </c>
     </row>
     <row r="655">
@@ -12318,7 +12318,7 @@
         <v>9.00027376028493</v>
       </c>
       <c r="E655" t="n">
-        <v>9.00027376028493</v>
+        <v>8.94728365888591</v>
       </c>
     </row>
     <row r="656">
@@ -12335,7 +12335,7 @@
         <v>18.7476379570928</v>
       </c>
       <c r="E656" t="n">
-        <v>18.7476379570928</v>
+        <v>18.8171807360682</v>
       </c>
     </row>
     <row r="657">
@@ -12352,7 +12352,7 @@
         <v>17.0283550648801</v>
       </c>
       <c r="E657" t="n">
-        <v>17.0283550648801</v>
+        <v>17.0915203092325</v>
       </c>
     </row>
     <row r="658">
@@ -12369,7 +12369,7 @@
         <v>17.3995366251834</v>
       </c>
       <c r="E658" t="n">
-        <v>17.3995366251834</v>
+        <v>17.464078736172</v>
       </c>
     </row>
     <row r="659">
@@ -12386,7 +12386,7 @@
         <v>17.1401196216136</v>
       </c>
       <c r="E659" t="n">
-        <v>17.1401196216136</v>
+        <v>17.2036994471464</v>
       </c>
     </row>
     <row r="660">
@@ -12403,7 +12403,7 @@
         <v>-1.47273871692278</v>
       </c>
       <c r="E660" t="n">
-        <v>-1.47273871692278</v>
+        <v>-1.47820171675858</v>
       </c>
     </row>
     <row r="661">
@@ -12420,7 +12420,7 @@
         <v>-1.45071082909249</v>
       </c>
       <c r="E661" t="n">
-        <v>-1.45071082909249</v>
+        <v>-1.45609211833971</v>
       </c>
     </row>
     <row r="662">
@@ -12505,7 +12505,7 @@
         <v>4.59568595523936</v>
       </c>
       <c r="E666" t="n">
-        <v>4.44101888500192</v>
+        <v>5.64253271687592</v>
       </c>
     </row>
     <row r="667">
@@ -12522,7 +12522,7 @@
         <v>12.4594257274391</v>
       </c>
       <c r="E667" t="n">
-        <v>12.3047586572017</v>
+        <v>13.4943497162609</v>
       </c>
     </row>
     <row r="668">
@@ -12539,7 +12539,7 @@
         <v>9.20112169008648</v>
       </c>
       <c r="E668" t="n">
-        <v>9.04645461984904</v>
+        <v>10.2516928041777</v>
       </c>
     </row>
     <row r="669">
@@ -12556,7 +12556,7 @@
         <v>10.2737110932456</v>
       </c>
       <c r="E669" t="n">
-        <v>10.2737110932456</v>
+        <v>11.4931614575535</v>
       </c>
     </row>
     <row r="670">
@@ -12573,7 +12573,7 @@
         <v>13.9895557666743</v>
       </c>
       <c r="E670" t="n">
-        <v>13.9895557666743</v>
+        <v>14.0220142740807</v>
       </c>
     </row>
     <row r="671">
@@ -12590,7 +12590,7 @@
         <v>15.8210210854732</v>
       </c>
       <c r="E671" t="n">
-        <v>15.8210210854732</v>
+        <v>15.8797078264393</v>
       </c>
     </row>
     <row r="672">
@@ -12607,7 +12607,7 @@
         <v>11.2714363338197</v>
       </c>
       <c r="E672" t="n">
-        <v>11.2714363338197</v>
+        <v>11.3132467745533</v>
       </c>
     </row>
     <row r="673">
@@ -12624,7 +12624,7 @@
         <v>7.11364650767589</v>
       </c>
       <c r="E673" t="n">
-        <v>7.11364650767589</v>
+        <v>7.14003397834953</v>
       </c>
     </row>
     <row r="674">
@@ -14749,7 +14749,7 @@
         <v>0.173958065935262</v>
       </c>
       <c r="E798" t="n">
-        <v>0.173862653551516</v>
+        <v>0.115908435701011</v>
       </c>
     </row>
     <row r="799">
@@ -14766,7 +14766,7 @@
         <v>0.0843877416588816</v>
       </c>
       <c r="E799" t="n">
-        <v>0.084341456736436</v>
+        <v>0.113593778501241</v>
       </c>
     </row>
     <row r="800">
@@ -14783,7 +14783,7 @@
         <v>-0.00233393479700826</v>
       </c>
       <c r="E800" t="n">
-        <v>-0.00233265468227893</v>
+        <v>0.0355820679506332</v>
       </c>
     </row>
     <row r="801">
@@ -14800,7 +14800,7 @@
         <v>0.229743120072647</v>
       </c>
       <c r="E801" t="n">
-        <v>0.229617110746104</v>
+        <v>0.139817184401413</v>
       </c>
     </row>
     <row r="802">
@@ -14817,7 +14817,7 @@
         <v>0.112487146913513</v>
       </c>
       <c r="E802" t="n">
-        <v>0.112425450051283</v>
+        <v>0.145998199232411</v>
       </c>
     </row>
     <row r="803">
@@ -14834,7 +14834,7 @@
         <v>0.128467766460149</v>
       </c>
       <c r="E803" t="n">
-        <v>0.128397304560227</v>
+        <v>0.141173774832674</v>
       </c>
     </row>
     <row r="804">
@@ -14851,7 +14851,7 @@
         <v>0.076927590310909</v>
       </c>
       <c r="E804" t="n">
-        <v>0.0768853971264314</v>
+        <v>0.0772109596872256</v>
       </c>
     </row>
     <row r="805">
@@ -14868,7 +14868,7 @@
         <v>-0.216227465807936</v>
       </c>
       <c r="E805" t="n">
-        <v>-0.216108869536857</v>
+        <v>-0.11865878495587</v>
       </c>
     </row>
     <row r="806">
@@ -15157,7 +15157,7 @@
         <v>9.58896</v>
       </c>
       <c r="E822" t="n">
-        <v>9.58896</v>
+        <v>6.39264</v>
       </c>
     </row>
     <row r="823">
@@ -15174,7 +15174,7 @@
         <v>4.69932754434226</v>
       </c>
       <c r="E823" t="n">
-        <v>4.69932754434226</v>
+        <v>6.3292050295615</v>
       </c>
     </row>
     <row r="824">
@@ -15191,7 +15191,7 @@
         <v>-0.13185229589659</v>
       </c>
       <c r="E824" t="n">
-        <v>-0.13185229589659</v>
+        <v>2.01126098418303</v>
       </c>
     </row>
     <row r="825">
@@ -15208,7 +15208,7 @@
         <v>13.1515434572293</v>
       </c>
       <c r="E825" t="n">
-        <v>13.1515434572293</v>
+        <v>8.00816529198415</v>
       </c>
     </row>
     <row r="826">
@@ -15225,7 +15225,7 @@
         <v>6.51921396217004</v>
       </c>
       <c r="E826" t="n">
-        <v>6.51921396217004</v>
+        <v>8.46599678679032</v>
       </c>
     </row>
     <row r="827">
@@ -15242,7 +15242,7 @@
         <v>7.52075473287565</v>
       </c>
       <c r="E827" t="n">
-        <v>7.52075473287565</v>
+        <v>8.26912479874317</v>
       </c>
     </row>
     <row r="828">
@@ -15259,7 +15259,7 @@
         <v>4.55194904329692</v>
       </c>
       <c r="E828" t="n">
-        <v>4.55194904329692</v>
+        <v>4.57122375920564</v>
       </c>
     </row>
     <row r="829">
@@ -15276,7 +15276,7 @@
         <v>-12.9289856334763</v>
       </c>
       <c r="E829" t="n">
-        <v>-12.9289856334763</v>
+        <v>-7.09891143879473</v>
       </c>
     </row>
     <row r="830">
@@ -19441,7 +19441,7 @@
         <v>1874.84887398125</v>
       </c>
       <c r="E1074" t="n">
-        <v>1871.51823548271</v>
+        <v>1918.5942369875</v>
       </c>
     </row>
     <row r="1075">
@@ -19458,7 +19458,7 @@
         <v>1686.46750742639</v>
       </c>
       <c r="E1075" t="n">
-        <v>1683.33707345659</v>
+        <v>1729.8847802101</v>
       </c>
     </row>
     <row r="1076">
@@ -19475,7 +19475,7 @@
         <v>1683.04452003779</v>
       </c>
       <c r="E1076" t="n">
-        <v>1679.85922632371</v>
+        <v>1727.11305191325</v>
       </c>
     </row>
     <row r="1077">
@@ -19492,7 +19492,7 @@
         <v>1684.5361789841</v>
       </c>
       <c r="E1077" t="n">
-        <v>1681.31110886363</v>
+        <v>1728.60153200657</v>
       </c>
     </row>
     <row r="1078">
@@ -19509,7 +19509,7 @@
         <v>1678.21355365355</v>
       </c>
       <c r="E1078" t="n">
-        <v>1674.95812042381</v>
+        <v>1722.06497564255</v>
       </c>
     </row>
     <row r="1079">
@@ -19526,7 +19526,7 @@
         <v>1660.19846222559</v>
       </c>
       <c r="E1079" t="n">
-        <v>1656.92675094587</v>
+        <v>1703.5206059736</v>
       </c>
     </row>
     <row r="1080">
@@ -19543,7 +19543,7 @@
         <v>1681.586301789</v>
       </c>
       <c r="E1080" t="n">
-        <v>1678.26358458777</v>
+        <v>1725.45642803293</v>
       </c>
     </row>
     <row r="1081">
@@ -19560,7 +19560,7 @@
         <v>1692.73756326328</v>
       </c>
       <c r="E1081" t="n">
-        <v>1689.37617139796</v>
+        <v>1736.87959026913</v>
       </c>
     </row>
     <row r="1082">
@@ -19645,7 +19645,7 @@
         <v>0.5109043988589</v>
       </c>
       <c r="E1086" t="n">
-        <v>0.510624178414397</v>
+        <v>0.452669960563891</v>
       </c>
     </row>
     <row r="1087">
@@ -19662,7 +19662,7 @@
         <v>0.414605355911433</v>
       </c>
       <c r="E1087" t="n">
-        <v>0.414377953490576</v>
+        <v>0.443630275255381</v>
       </c>
     </row>
     <row r="1088">
@@ -19679,7 +19679,7 @@
         <v>0.296798150081424</v>
       </c>
       <c r="E1088" t="n">
-        <v>0.296635362464544</v>
+        <v>0.334550085097456</v>
       </c>
     </row>
     <row r="1089">
@@ -19696,7 +19696,7 @@
         <v>0.491926631727405</v>
       </c>
       <c r="E1089" t="n">
-        <v>0.491656820193753</v>
+        <v>0.401856893849062</v>
       </c>
     </row>
     <row r="1090">
@@ -19713,7 +19713,7 @@
         <v>0.0485562976155232</v>
       </c>
       <c r="E1090" t="n">
-        <v>0.0485296654954403</v>
+        <v>0.0821024146765683</v>
       </c>
     </row>
     <row r="1091">
@@ -19730,7 +19730,7 @@
         <v>-0.0374583419229707</v>
       </c>
       <c r="E1091" t="n">
-        <v>-0.0374377968009332</v>
+        <v>-0.0246613265284864</v>
       </c>
     </row>
     <row r="1092">
@@ -19747,7 +19747,7 @@
         <v>0.0374191809270202</v>
       </c>
       <c r="E1092" t="n">
-        <v>0.0373986572839752</v>
+        <v>0.0377242198447694</v>
       </c>
     </row>
     <row r="1093">
@@ -19764,7 +19764,7 @@
         <v>-0.307229467273953</v>
       </c>
       <c r="E1093" t="n">
-        <v>-0.30706095829639</v>
+        <v>-0.209610873715403</v>
       </c>
     </row>
     <row r="1094">
@@ -19849,7 +19849,7 @@
         <v>-0.133200161525696</v>
       </c>
       <c r="E1098" t="n">
-        <v>-0.150172653319984</v>
+        <v>0.0418784837740344</v>
       </c>
     </row>
     <row r="1099">
@@ -19866,7 +19866,7 @@
         <v>-1.00170560942911</v>
       </c>
       <c r="E1099" t="n">
-        <v>-1.01708684822963</v>
+        <v>-0.831004275808255</v>
       </c>
     </row>
     <row r="1100">
@@ -19883,7 +19883,7 @@
         <v>-0.580879065281866</v>
       </c>
       <c r="E1100" t="n">
-        <v>-0.596372622378126</v>
+        <v>-0.411763403164291</v>
       </c>
     </row>
     <row r="1101">
@@ -19900,7 +19900,7 @@
         <v>-0.746819922693185</v>
       </c>
       <c r="E1101" t="n">
-        <v>-0.744452399775073</v>
+        <v>-0.563934917801284</v>
       </c>
     </row>
     <row r="1102">
@@ -19917,7 +19917,7 @@
         <v>-1.01795355860441</v>
       </c>
       <c r="E1102" t="n">
-        <v>-1.01663105869443</v>
+        <v>-1.02341264539197</v>
       </c>
     </row>
     <row r="1103">
@@ -19934,7 +19934,7 @@
         <v>-0.341428343063879</v>
       </c>
       <c r="E1103" t="n">
-        <v>-0.341326829223745</v>
+        <v>-0.347869597860318</v>
       </c>
     </row>
     <row r="1104">
@@ -19951,7 +19951,7 @@
         <v>-0.246729671779656</v>
       </c>
       <c r="E1104" t="n">
-        <v>-0.24665163362289</v>
+        <v>-0.25365002359298</v>
       </c>
     </row>
     <row r="1105">
@@ -19968,7 +19968,7 @@
         <v>-0.205127762370454</v>
       </c>
       <c r="E1105" t="n">
-        <v>-0.205067956755791</v>
+        <v>-0.210887050368215</v>
       </c>
     </row>
     <row r="1106">
@@ -20461,7 +20461,7 @@
         <v>50.1764906511619</v>
       </c>
       <c r="E1134" t="n">
-        <v>50.4776432622514</v>
+        <v>97.5536447670418</v>
       </c>
     </row>
     <row r="1135">
@@ -20478,7 +20478,7 @@
         <v>-206.985727647878</v>
       </c>
       <c r="E1135" t="n">
-        <v>-206.752472774563</v>
+        <v>-207.747908607441</v>
       </c>
     </row>
     <row r="1136">
@@ -20495,7 +20495,7 @@
         <v>-18.2451214312764</v>
       </c>
       <c r="E1136" t="n">
-        <v>-18.2724682162511</v>
+        <v>-17.9754508576182</v>
       </c>
     </row>
     <row r="1137">
@@ -20512,7 +20512,7 @@
         <v>-14.9517601915684</v>
       </c>
       <c r="E1137" t="n">
-        <v>-14.9604161379837</v>
+        <v>-15.3854905432174</v>
       </c>
     </row>
     <row r="1138">
@@ -20529,7 +20529,7 @@
         <v>-22.0204654482416</v>
       </c>
       <c r="E1138" t="n">
-        <v>-22.0207748039927</v>
+        <v>-22.6450322846813</v>
       </c>
     </row>
     <row r="1139">
@@ -20546,7 +20546,7 @@
         <v>-33.6176933887268</v>
       </c>
       <c r="E1139" t="n">
-        <v>-33.60370518994</v>
+        <v>-34.5546648468332</v>
       </c>
     </row>
     <row r="1140">
@@ -20563,7 +20563,7 @@
         <v>5.70345233830881</v>
       </c>
       <c r="E1140" t="n">
-        <v>5.68335524352233</v>
+        <v>5.84215769451566</v>
       </c>
     </row>
     <row r="1141">
@@ -20580,7 +20580,7 @@
         <v>-4.57772060480056</v>
       </c>
       <c r="E1141" t="n">
-        <v>-4.58531571070239</v>
+        <v>-4.71616597186653</v>
       </c>
     </row>
     <row r="1142">
@@ -20665,7 +20665,7 @@
         <v>-7.34229260365982</v>
       </c>
       <c r="E1146" t="n">
-        <v>-8.2823972622304</v>
+        <v>2.30970307634743</v>
       </c>
     </row>
     <row r="1147">
@@ -20682,7 +20682,7 @@
         <v>-55.782305216091</v>
       </c>
       <c r="E1147" t="n">
-        <v>-56.6699275281657</v>
+        <v>-46.3018002519853</v>
       </c>
     </row>
     <row r="1148">
@@ -20699,7 +20699,7 @@
         <v>-32.8159289170614</v>
       </c>
       <c r="E1148" t="n">
-        <v>-33.7097042557555</v>
+        <v>-23.2747480738827</v>
       </c>
     </row>
     <row r="1149">
@@ -20716,7 +20716,7 @@
         <v>-42.7513766894012</v>
       </c>
       <c r="E1149" t="n">
-        <v>-42.639235619973</v>
+        <v>-32.2999211792778</v>
       </c>
     </row>
     <row r="1150">
@@ -20733,7 +20733,7 @@
         <v>-58.995691811767</v>
       </c>
       <c r="E1150" t="n">
-        <v>-58.9513796848779</v>
+        <v>-59.3446235159155</v>
       </c>
     </row>
     <row r="1151">
@@ -20750,7 +20750,7 @@
         <v>-19.987884103458</v>
       </c>
       <c r="E1151" t="n">
-        <v>-19.9929069783377</v>
+        <v>-20.3761436697788</v>
       </c>
     </row>
     <row r="1152">
@@ -20767,7 +20767,7 @@
         <v>-14.5994550053013</v>
       </c>
       <c r="E1152" t="n">
-        <v>-14.6028466998887</v>
+        <v>-15.0171817455487</v>
       </c>
     </row>
     <row r="1153">
@@ -20784,7 +20784,7 @@
         <v>-12.2652960982785</v>
       </c>
       <c r="E1153" t="n">
-        <v>-12.2684491037504</v>
+        <v>-12.6165837169947</v>
       </c>
     </row>
     <row r="1154">
@@ -20869,7 +20869,7 @@
         <v>847.383583333333</v>
       </c>
       <c r="E1158" t="n">
-        <v>847.785457935954</v>
+        <v>847.383583333333</v>
       </c>
     </row>
     <row r="1159">
@@ -20886,7 +20886,7 @@
         <v>107.416916666667</v>
       </c>
       <c r="E1159" t="n">
-        <v>107.820708942648</v>
+        <v>107.416916666667</v>
       </c>
     </row>
     <row r="1160">
@@ -20903,7 +20903,7 @@
         <v>102.75025</v>
       </c>
       <c r="E1160" t="n">
-        <v>103.155998918104</v>
+        <v>102.75025</v>
       </c>
     </row>
     <row r="1161">
@@ -20920,7 +20920,7 @@
         <v>77.3302500000004</v>
       </c>
       <c r="E1161" t="n">
-        <v>77.7379781210906</v>
+        <v>77.3302499999996</v>
       </c>
     </row>
     <row r="1162">
@@ -20937,7 +20937,7 @@
         <v>77.703294275287</v>
       </c>
       <c r="E1162" t="n">
-        <v>78.1129892934381</v>
+        <v>77.703294275287</v>
       </c>
     </row>
     <row r="1163">
@@ -20954,7 +20954,7 @@
         <v>78.0705036557577</v>
       </c>
       <c r="E1163" t="n">
-        <v>78.4821348061566</v>
+        <v>78.0705036557575</v>
       </c>
     </row>
     <row r="1164">
@@ -20971,7 +20971,7 @@
         <v>78.4353790783013</v>
       </c>
       <c r="E1164" t="n">
-        <v>78.8489340550226</v>
+        <v>78.4353790783014</v>
       </c>
     </row>
     <row r="1165">
@@ -20988,7 +20988,7 @@
         <v>78.7994765148695</v>
       </c>
       <c r="E1165" t="n">
-        <v>79.2149512159381</v>
+        <v>78.7994765148698</v>
       </c>
     </row>
     <row r="1166">
@@ -21260,7 +21260,7 @@
         <v>0.506308345731002</v>
       </c>
       <c r="E1181" t="n">
-        <v>0.505860862391329</v>
+        <v>0.448888874076566</v>
       </c>
     </row>
     <row r="1182">
@@ -21277,7 +21277,7 @@
         <v>0.511745955104348</v>
       </c>
       <c r="E1182" t="n">
-        <v>0.511712095978281</v>
+        <v>0.479820055014627</v>
       </c>
     </row>
     <row r="1183">
@@ -21294,7 +21294,7 @@
         <v>-0.54188338943326</v>
       </c>
       <c r="E1183" t="n">
-        <v>-0.541450820305582</v>
+        <v>-0.186354559738072</v>
       </c>
     </row>
     <row r="1184">
@@ -21311,7 +21311,7 @@
         <v>-0.247937055134324</v>
       </c>
       <c r="E1184" t="n">
-        <v>-0.247680344971713</v>
+        <v>-0.0962484779176302</v>
       </c>
     </row>
     <row r="1185">
@@ -21328,7 +21328,7 @@
         <v>-0.213119054454151</v>
       </c>
       <c r="E1185" t="n">
-        <v>-0.212896029199773</v>
+        <v>-0.0911247951814319</v>
       </c>
     </row>
     <row r="1186">
@@ -21345,7 +21345,7 @@
         <v>-0.234860432492177</v>
       </c>
       <c r="E1186" t="n">
-        <v>-0.234673665274137</v>
+        <v>-0.0942256277902956</v>
       </c>
     </row>
     <row r="1187">
@@ -21362,7 +21362,7 @@
         <v>-0.169416115484793</v>
       </c>
       <c r="E1187" t="n">
-        <v>-0.169267093242703</v>
+        <v>-0.079633956373134</v>
       </c>
     </row>
     <row r="1188">
@@ -21379,7 +21379,7 @@
         <v>-0.0955356666981516</v>
       </c>
       <c r="E1188" t="n">
-        <v>-0.0954291548065742</v>
+        <v>-0.0536237460885096</v>
       </c>
     </row>
     <row r="1189">
@@ -21396,7 +21396,7 @@
         <v>-0.10311970215545</v>
       </c>
       <c r="E1189" t="n">
-        <v>-0.102977392511377</v>
+        <v>-0.0536393382913875</v>
       </c>
     </row>
     <row r="1190">
@@ -21889,7 +21889,7 @@
         <v>87.7339429023295</v>
       </c>
       <c r="E1218" t="n">
-        <v>88.1358175049506</v>
+        <v>87.7339429023297</v>
       </c>
     </row>
     <row r="1219">
@@ -21906,7 +21906,7 @@
         <v>-748.375360501892</v>
       </c>
       <c r="E1219" t="n">
-        <v>-748.37743068074</v>
+        <v>-748.375360501892</v>
       </c>
     </row>
     <row r="1220">
@@ -21923,7 +21923,7 @@
         <v>-5.61073936908998</v>
       </c>
       <c r="E1220" t="n">
-        <v>-5.61233160247941</v>
+        <v>-5.61073936908976</v>
       </c>
     </row>
     <row r="1221">
@@ -21940,7 +21940,7 @@
         <v>-26.4238744710284</v>
       </c>
       <c r="E1221" t="n">
-        <v>-26.4258594528547</v>
+        <v>-26.4238744710293</v>
       </c>
     </row>
     <row r="1222">
@@ -21957,7 +21957,7 @@
         <v>-0.347580141040225</v>
       </c>
       <c r="E1222" t="n">
-        <v>-0.349412777011722</v>
+        <v>-0.347580141039415</v>
       </c>
     </row>
     <row r="1223">
@@ -21974,7 +21974,7 @@
         <v>-0.355209747284334</v>
       </c>
       <c r="E1223" t="n">
-        <v>-0.35708261078662</v>
+        <v>-0.355209747284505</v>
       </c>
     </row>
     <row r="1224">
@@ -21991,7 +21991,7 @@
         <v>-0.372679778269216</v>
       </c>
       <c r="E1224" t="n">
-        <v>-0.374644753499012</v>
+        <v>-0.372679778268932</v>
       </c>
     </row>
     <row r="1225">
@@ -22008,7 +22008,7 @@
         <v>-0.369560223806232</v>
       </c>
       <c r="E1225" t="n">
-        <v>-0.371508751008506</v>
+        <v>-0.369560223806062</v>
       </c>
     </row>
     <row r="1226">
@@ -22076,7 +22076,7 @@
         <v>27.2073649974604</v>
       </c>
       <c r="E1229" t="n">
-        <v>27.1833186971072</v>
+        <v>24.1218292040339</v>
       </c>
     </row>
     <row r="1230">
@@ -22093,7 +22093,7 @@
         <v>28.2085884737506</v>
       </c>
       <c r="E1230" t="n">
-        <v>28.2222013734422</v>
+        <v>26.4632755841942</v>
       </c>
     </row>
     <row r="1231">
@@ -22110,7 +22110,7 @@
         <v>-30.1760360892091</v>
       </c>
       <c r="E1231" t="n">
-        <v>-30.1684942639782</v>
+        <v>-10.3832818340754</v>
       </c>
     </row>
     <row r="1232">
@@ -22127,7 +22127,7 @@
         <v>-14.0068480058676</v>
       </c>
       <c r="E1232" t="n">
-        <v>-14.0000242560869</v>
+        <v>-5.4404035395387</v>
       </c>
     </row>
     <row r="1233">
@@ -22144,7 +22144,7 @@
         <v>-12.199906161852</v>
       </c>
       <c r="E1233" t="n">
-        <v>-12.1938272404636</v>
+        <v>-5.21926131709268</v>
       </c>
     </row>
     <row r="1234">
@@ -22161,7 +22161,7 @@
         <v>-13.6113809681875</v>
       </c>
       <c r="E1234" t="n">
-        <v>-13.6080205550515</v>
+        <v>-5.4638609674636</v>
       </c>
     </row>
     <row r="1235">
@@ -22178,7 +22178,7 @@
         <v>-9.91795130767616</v>
       </c>
       <c r="E1235" t="n">
-        <v>-9.91466524149677</v>
+        <v>-4.66448619262043</v>
       </c>
     </row>
     <row r="1236">
@@ -22195,7 +22195,7 @@
         <v>-5.65302364041053</v>
       </c>
       <c r="E1236" t="n">
-        <v>-5.64981994188187</v>
+        <v>-3.17475839143029</v>
       </c>
     </row>
     <row r="1237">
@@ -22212,7 +22212,7 @@
         <v>-6.16588250116388</v>
       </c>
       <c r="E1237" t="n">
-        <v>-6.16075236155627</v>
+        <v>-3.20904105252491</v>
       </c>
     </row>
     <row r="1238">
@@ -22484,7 +22484,7 @@
         <v>8.92592515030801</v>
       </c>
       <c r="E1253" t="n">
-        <v>8.76929541766614</v>
+        <v>7.20720821490317</v>
       </c>
     </row>
     <row r="1254">
@@ -22501,7 +22501,7 @@
         <v>-1.1116744369821</v>
       </c>
       <c r="E1254" t="n">
-        <v>-1.21759223016378</v>
+        <v>0.871027662755511</v>
       </c>
     </row>
     <row r="1255">
@@ -22518,7 +22518,7 @@
         <v>-2.37393965461218</v>
       </c>
       <c r="E1255" t="n">
-        <v>-2.47005208949594</v>
+        <v>-2.18679562664528</v>
       </c>
     </row>
     <row r="1256">
@@ -22535,7 +22535,7 @@
         <v>-1.90956443405137</v>
       </c>
       <c r="E1256" t="n">
-        <v>-2.00199233034765</v>
+        <v>-1.92753705917553</v>
       </c>
     </row>
     <row r="1257">
@@ -22552,7 +22552,7 @@
         <v>-0.898679473996908</v>
       </c>
       <c r="E1257" t="n">
-        <v>-0.975103753443741</v>
+        <v>-0.858694674702927</v>
       </c>
     </row>
     <row r="1258">
@@ -22569,7 +22569,7 @@
         <v>-4.04976996715075</v>
       </c>
       <c r="E1258" t="n">
-        <v>-4.12563272865071</v>
+        <v>-3.95555400574937</v>
       </c>
     </row>
     <row r="1259">
@@ -22586,7 +22586,7 @@
         <v>-2.67536216832743</v>
       </c>
       <c r="E1259" t="n">
-        <v>-2.75539545906091</v>
+        <v>-2.51503369724652</v>
       </c>
     </row>
     <row r="1260">
@@ -22603,7 +22603,7 @@
         <v>-0.978004478023472</v>
       </c>
       <c r="E1260" t="n">
-        <v>-1.00670972575284</v>
+        <v>-0.919054293167201</v>
       </c>
     </row>
     <row r="1261">
@@ -22620,7 +22620,7 @@
         <v>-1.76737565231144</v>
       </c>
       <c r="E1261" t="n">
-        <v>-1.78286321018272</v>
+        <v>-1.64090067663189</v>
       </c>
     </row>
     <row r="1262">
@@ -22688,7 +22688,7 @@
         <v>4.51534564334464</v>
       </c>
       <c r="E1265" t="n">
-        <v>4.51534564334464</v>
+        <v>3.01023042889643</v>
       </c>
     </row>
     <row r="1266">
@@ -22705,7 +22705,7 @@
         <v>0.893739003957893</v>
       </c>
       <c r="E1266" t="n">
-        <v>0.893248806689053</v>
+        <v>2.79992430214306</v>
       </c>
     </row>
     <row r="1267">
@@ -22722,7 +22722,7 @@
         <v>1.8601681512636</v>
       </c>
       <c r="E1267" t="n">
-        <v>1.85914788769303</v>
+        <v>1.57987526224807</v>
       </c>
     </row>
     <row r="1268">
@@ -22739,7 +22739,7 @@
         <v>0.0598457574973709</v>
       </c>
       <c r="E1268" t="n">
-        <v>0.0598129333431749</v>
+        <v>-0.22309525975763</v>
       </c>
     </row>
     <row r="1269">
@@ -22756,7 +22756,7 @@
         <v>0.971586576418761</v>
       </c>
       <c r="E1269" t="n">
-        <v>0.971053681374353</v>
+        <v>0.763883260249547</v>
       </c>
     </row>
     <row r="1270">
@@ -22773,7 +22773,7 @@
         <v>-1.18588421759819</v>
       </c>
       <c r="E1270" t="n">
-        <v>-1.1852337847514</v>
+        <v>-1.14938126758908</v>
       </c>
     </row>
     <row r="1271">
@@ -22790,7 +22790,7 @@
         <v>-1.54948525202102</v>
       </c>
       <c r="E1271" t="n">
-        <v>-1.54863539156368</v>
+        <v>-1.39236592127604</v>
       </c>
     </row>
     <row r="1272">
@@ -22807,7 +22807,7 @@
         <v>-0.338724905299275</v>
       </c>
       <c r="E1272" t="n">
-        <v>-0.338539121728534</v>
+        <v>-0.286396913586333</v>
       </c>
     </row>
     <row r="1273">
@@ -22824,7 +22824,7 @@
         <v>-0.655214610312738</v>
       </c>
       <c r="E1273" t="n">
-        <v>-0.654855238716492</v>
+        <v>-0.556852734130703</v>
       </c>
     </row>
     <row r="1274">
@@ -22892,7 +22892,7 @@
         <v>8.83086719529685</v>
       </c>
       <c r="E1277" t="n">
-        <v>8.81766109847841</v>
+        <v>7.25557389571543</v>
       </c>
     </row>
     <row r="1278">
@@ -22909,7 +22909,7 @@
         <v>-1.22471293947181</v>
       </c>
       <c r="E1278" t="n">
-        <v>-1.24440161328137</v>
+        <v>0.844218279637919</v>
       </c>
     </row>
     <row r="1279">
@@ -22926,7 +22926,7 @@
         <v>-2.49998762573205</v>
       </c>
       <c r="E1279" t="n">
-        <v>-2.52405695171762</v>
+        <v>-2.24080048886697</v>
       </c>
     </row>
     <row r="1280">
@@ -22943,7 +22943,7 @@
         <v>-1.90058987275835</v>
       </c>
       <c r="E1280" t="n">
-        <v>-1.9181874321962</v>
+        <v>-1.84373216102408</v>
       </c>
     </row>
     <row r="1281">
@@ -22960,7 +22960,7 @@
         <v>-0.73618113323843</v>
       </c>
       <c r="E1281" t="n">
-        <v>-0.735113874833972</v>
+        <v>-0.618704796093159</v>
       </c>
     </row>
     <row r="1282">
@@ -22977,7 +22977,7 @@
         <v>-3.53137209960125</v>
       </c>
       <c r="E1282" t="n">
-        <v>-3.52871776166035</v>
+        <v>-3.35863903875901</v>
       </c>
     </row>
     <row r="1283">
@@ -22994,7 +22994,7 @@
         <v>-2.17814133527343</v>
       </c>
       <c r="E1283" t="n">
-        <v>-2.17824461744353</v>
+        <v>-1.93788285562914</v>
       </c>
     </row>
     <row r="1284">
@@ -23011,7 +23011,7 @@
         <v>-0.583142209253553</v>
       </c>
       <c r="E1284" t="n">
-        <v>-0.582827911428223</v>
+        <v>-0.495172478842585</v>
       </c>
     </row>
     <row r="1285">
@@ -23028,7 +23028,7 @@
         <v>-1.39787754724436</v>
       </c>
       <c r="E1285" t="n">
-        <v>-1.39707779253135</v>
+        <v>-1.25511525898051</v>
       </c>
     </row>
     <row r="1286">
@@ -23334,7 +23334,7 @@
         <v>425.20704</v>
       </c>
       <c r="E1303" t="n">
-        <v>425.20704</v>
+        <v>350</v>
       </c>
     </row>
     <row r="1304">
@@ -23538,7 +23538,7 @@
         <v>1.05837859219536</v>
       </c>
       <c r="E1315" t="n">
-        <v>1.05779809353412</v>
+        <v>0.868828506911009</v>
       </c>
     </row>
     <row r="1316">
@@ -23555,7 +23555,7 @@
         <v>0.431881345247741</v>
       </c>
       <c r="E1316" t="n">
-        <v>0.431644467305785</v>
+        <v>0.433281593079357</v>
       </c>
     </row>
     <row r="1317">
@@ -23572,7 +23572,7 @@
         <v>0.421792993256423</v>
       </c>
       <c r="E1317" t="n">
-        <v>0.421561648565865</v>
+        <v>0.344393434117818</v>
       </c>
     </row>
     <row r="1318">
@@ -23589,7 +23589,7 @@
         <v>-0.834507978480187</v>
       </c>
       <c r="E1318" t="n">
-        <v>-0.834050268197806</v>
+        <v>-0.831770500216609</v>
       </c>
     </row>
     <row r="1319">
@@ -23606,7 +23606,7 @@
         <v>-1.1087469368494</v>
       </c>
       <c r="E1319" t="n">
-        <v>-1.10813881219793</v>
+        <v>-0.964645812182739</v>
       </c>
     </row>
     <row r="1320">
@@ -23623,7 +23623,7 @@
         <v>-0.296688102735558</v>
       </c>
       <c r="E1320" t="n">
-        <v>-0.29652537547736</v>
+        <v>-0.244708729895953</v>
       </c>
     </row>
     <row r="1321">
@@ -23640,7 +23640,7 @@
         <v>-0.0777659440213239</v>
       </c>
       <c r="E1321" t="n">
-        <v>-0.0777232910172598</v>
+        <v>-0.0771708710124585</v>
       </c>
     </row>
     <row r="1322">
@@ -23742,7 +23742,7 @@
         <v>-4.21938291732999</v>
       </c>
       <c r="E1327" t="n">
-        <v>-4.21938291732999</v>
+        <v>-79.42642291733</v>
       </c>
     </row>
     <row r="1328">
@@ -23759,7 +23759,7 @@
         <v>-428.944126967295</v>
       </c>
       <c r="E1328" t="n">
-        <v>-428.944126967295</v>
+        <v>-353.07610249951</v>
       </c>
     </row>
     <row r="1329">
@@ -23946,7 +23946,7 @@
         <v>58.9382719915738</v>
       </c>
       <c r="E1339" t="n">
-        <v>58.9382719915738</v>
+        <v>48.4092863915738</v>
       </c>
     </row>
     <row r="1340">
@@ -23963,7 +23963,7 @@
         <v>24.3985166161525</v>
       </c>
       <c r="E1340" t="n">
-        <v>24.3985166161525</v>
+        <v>24.4910544416424</v>
       </c>
     </row>
     <row r="1341">
@@ -23980,7 +23980,7 @@
         <v>24.1453536411127</v>
       </c>
       <c r="E1341" t="n">
-        <v>24.1453536411127</v>
+        <v>19.7254690666026</v>
       </c>
     </row>
     <row r="1342">
@@ -23997,7 +23997,7 @@
         <v>-48.364068376925</v>
       </c>
       <c r="E1342" t="n">
-        <v>-48.364068376925</v>
+        <v>-48.231871483368</v>
       </c>
     </row>
     <row r="1343">
@@ -24014,7 +24014,7 @@
         <v>-64.9082178560187</v>
       </c>
       <c r="E1343" t="n">
-        <v>-64.9082178560187</v>
+        <v>-56.5032465624617</v>
       </c>
     </row>
     <row r="1344">
@@ -24031,7 +24031,7 @@
         <v>-17.555588572923</v>
       </c>
       <c r="E1344" t="n">
-        <v>-17.555588572923</v>
+        <v>-14.4878183708224</v>
       </c>
     </row>
     <row r="1345">
@@ -24048,7 +24048,7 @@
         <v>-4.64989389423125</v>
       </c>
       <c r="E1345" t="n">
-        <v>-4.64989389423125</v>
+        <v>-4.616844670842</v>
       </c>
     </row>
     <row r="1346">
@@ -24932,7 +24932,7 @@
         <v>9.29130159787437</v>
       </c>
       <c r="E1397" t="n">
-        <v>9.04588759951116</v>
+        <v>7.48277501367665</v>
       </c>
     </row>
     <row r="1398">
@@ -24949,7 +24949,7 @@
         <v>-0.0551593346690562</v>
       </c>
       <c r="E1398" t="n">
-        <v>-0.147635030498831</v>
+        <v>1.9185923954209</v>
       </c>
     </row>
     <row r="1399">
@@ -24966,7 +24966,7 @@
         <v>-1.6782382452802</v>
       </c>
       <c r="E1399" t="n">
-        <v>-1.74674459010501</v>
+        <v>-1.48585891547859</v>
       </c>
     </row>
     <row r="1400">
@@ -24983,7 +24983,7 @@
         <v>-1.72158777153343</v>
       </c>
       <c r="E1400" t="n">
-        <v>-1.79287744916348</v>
+        <v>-1.74060339316573</v>
       </c>
     </row>
     <row r="1401">
@@ -25000,7 +25000,7 @@
         <v>-0.733392509410521</v>
       </c>
       <c r="E1401" t="n">
-        <v>-0.814538135839966</v>
+        <v>-0.720127163358024</v>
       </c>
     </row>
     <row r="1402">
@@ -25017,7 +25017,7 @@
         <v>-3.83003418259934</v>
       </c>
       <c r="E1402" t="n">
-        <v>-3.91214274640839</v>
+        <v>-3.74121175132524</v>
       </c>
     </row>
     <row r="1403">
@@ -25034,7 +25034,7 @@
         <v>-2.33853532110972</v>
       </c>
       <c r="E1403" t="n">
-        <v>-2.42342738676505</v>
+        <v>-2.18177542221658</v>
       </c>
     </row>
     <row r="1404">
@@ -25051,7 +25051,7 @@
         <v>-0.584490935643963</v>
       </c>
       <c r="E1404" t="n">
-        <v>-0.619297822659014</v>
+        <v>-0.529559547187543</v>
       </c>
     </row>
     <row r="1405">
@@ -25068,7 +25068,7 @@
         <v>-1.7415127221535</v>
       </c>
       <c r="E1405" t="n">
-        <v>-1.75691993751696</v>
+        <v>-1.61208156929698</v>
       </c>
     </row>
     <row r="1406">
@@ -25136,7 +25136,7 @@
         <v>5.89431513331637</v>
       </c>
       <c r="E1409" t="n">
-        <v>5.80535692335301</v>
+        <v>5.41457877689439</v>
       </c>
     </row>
     <row r="1410">
@@ -25153,7 +25153,7 @@
         <v>2.30782126349986</v>
       </c>
       <c r="E1410" t="n">
-        <v>2.19574412957906</v>
+        <v>2.32152283960037</v>
       </c>
     </row>
     <row r="1411">
@@ -25170,7 +25170,7 @@
         <v>1.0543134812303</v>
       </c>
       <c r="E1411" t="n">
-        <v>0.925109761103303</v>
+        <v>1.11610988978121</v>
       </c>
     </row>
     <row r="1412">
@@ -25187,7 +25187,7 @@
         <v>1.45907906159792</v>
       </c>
       <c r="E1412" t="n">
-        <v>1.33965763243596</v>
+        <v>1.54372627511331</v>
       </c>
     </row>
     <row r="1413">
@@ -25204,7 +25204,7 @@
         <v>-1.0470944652233</v>
       </c>
       <c r="E1413" t="n">
-        <v>-1.12544880140182</v>
+        <v>-0.506999269145363</v>
       </c>
     </row>
     <row r="1414">
@@ -25221,7 +25221,7 @@
         <v>-1.99081317720587</v>
       </c>
       <c r="E1414" t="n">
-        <v>-2.06657573037921</v>
+        <v>-1.9219503058319</v>
       </c>
     </row>
     <row r="1415">
@@ -25238,7 +25238,7 @@
         <v>-2.15588744616325</v>
       </c>
       <c r="E1415" t="n">
-        <v>-2.23574642954422</v>
+        <v>-2.09592943251639</v>
       </c>
     </row>
     <row r="1416">
@@ -25255,7 +25255,7 @@
         <v>-1.87161323719089</v>
       </c>
       <c r="E1416" t="n">
-        <v>-1.94235152291811</v>
+        <v>-1.79316847102185</v>
       </c>
     </row>
     <row r="1417">
@@ -25272,7 +25272,7 @@
         <v>-2.12364329037663</v>
       </c>
       <c r="E1417" t="n">
-        <v>-2.17794697333736</v>
+        <v>-2.01615707250659</v>
       </c>
     </row>
     <row r="1418">
@@ -26751,7 +26751,7 @@
         <v>-0.0336138006750541</v>
       </c>
       <c r="E1504" t="n">
-        <v>-0.0336138006750541</v>
+        <v>-0.0336515894640653</v>
       </c>
     </row>
     <row r="1505">
@@ -26768,7 +26768,7 @@
         <v>0.349563010759414</v>
       </c>
       <c r="E1505" t="n">
-        <v>0.345538160848326</v>
+        <v>0.345538896478206</v>
       </c>
     </row>
     <row r="1506">
@@ -26785,7 +26785,7 @@
         <v>-0.0786168969968658</v>
       </c>
       <c r="E1506" t="n">
-        <v>-0.0783254885740519</v>
+        <v>-0.0783251921351747</v>
       </c>
     </row>
     <row r="1507">
@@ -26802,7 +26802,7 @@
         <v>-0.178670744560466</v>
       </c>
       <c r="E1507" t="n">
-        <v>-0.178456659792065</v>
+        <v>-0.17845639711334</v>
       </c>
     </row>
     <row r="1508">
@@ -26819,7 +26819,7 @@
         <v>-0.0702922815703524</v>
       </c>
       <c r="E1508" t="n">
-        <v>-0.070237874391277</v>
+        <v>-0.0702376119718041</v>
       </c>
     </row>
     <row r="1509">
@@ -26836,7 +26836,7 @@
         <v>-0.232609178652863</v>
       </c>
       <c r="E1509" t="n">
-        <v>-0.232464227677992</v>
+        <v>-0.232463930597575</v>
       </c>
     </row>
     <row r="1510">
@@ -26853,7 +26853,7 @@
         <v>-0.0568379992333021</v>
       </c>
       <c r="E1510" t="n">
-        <v>-0.0567846407909642</v>
+        <v>-0.0567843409158527</v>
       </c>
     </row>
     <row r="1511">
@@ -26870,7 +26870,7 @@
         <v>-0.0567364999637957</v>
       </c>
       <c r="E1511" t="n">
-        <v>-0.0566826460559127</v>
+        <v>-0.056682346544087</v>
       </c>
     </row>
     <row r="1512">
@@ -26887,7 +26887,7 @@
         <v>-0.0568729941600924</v>
       </c>
       <c r="E1512" t="n">
-        <v>-0.0568191973167531</v>
+        <v>-0.0568188958152779</v>
       </c>
     </row>
     <row r="1513">
@@ -26904,7 +26904,7 @@
         <v>-0.0559690384203934</v>
       </c>
       <c r="E1513" t="n">
-        <v>-0.0559157552467441</v>
+        <v>-0.0559154587711852</v>
       </c>
     </row>
     <row r="1514">
@@ -39212,7 +39212,7 @@
         <v>4.51534564334464</v>
       </c>
       <c r="E2237" t="n">
-        <v>4.51534564334464</v>
+        <v>3.01023042889643</v>
       </c>
     </row>
     <row r="2238">
@@ -39229,7 +39229,7 @@
         <v>-1.49527134304354</v>
       </c>
       <c r="E2238" t="n">
-        <v>-1.49445121778853</v>
+        <v>0.470178495515984</v>
       </c>
     </row>
     <row r="2239">
@@ -39246,7 +39246,7 @@
         <v>-0.395037932152136</v>
       </c>
       <c r="E2239" t="n">
-        <v>-0.394821262056536</v>
+        <v>-0.514376622643195</v>
       </c>
     </row>
     <row r="2240">
@@ -39263,7 +39263,7 @@
         <v>-0.977013637987593</v>
       </c>
       <c r="E2240" t="n">
-        <v>-0.976477766312707</v>
+        <v>-1.29893780782</v>
       </c>
     </row>
     <row r="2241">
@@ -39280,7 +39280,7 @@
         <v>-0.173271015339701</v>
       </c>
       <c r="E2241" t="n">
-        <v>-0.173175979788928</v>
+        <v>-0.213378260120997</v>
       </c>
     </row>
     <row r="2242">
@@ -39620,7 +39620,7 @@
         <v>242.64</v>
       </c>
       <c r="E2261" t="n">
-        <v>242.64</v>
+        <v>161.76</v>
       </c>
     </row>
     <row r="2262">
@@ -39637,7 +39637,7 @@
         <v>-82.422720789082</v>
       </c>
       <c r="E2262" t="n">
-        <v>-82.422720789082</v>
+        <v>25.9315194739453</v>
       </c>
     </row>
     <row r="2263">
@@ -39654,7 +39654,7 @@
         <v>-21.9986054743196</v>
       </c>
       <c r="E2263" t="n">
-        <v>-21.9986054743196</v>
+        <v>-28.6599772459071</v>
       </c>
     </row>
     <row r="2264">
@@ -39671,7 +39671,7 @@
         <v>-55.1949829344303</v>
       </c>
       <c r="E2264" t="n">
-        <v>-55.1949829344303</v>
+        <v>-73.4218971582313</v>
       </c>
     </row>
     <row r="2265">
@@ -39688,7 +39688,7 @@
         <v>-9.91882275907874</v>
       </c>
       <c r="E2265" t="n">
-        <v>-9.91882275907874</v>
+        <v>-12.2214474857331</v>
       </c>
     </row>
     <row r="2266">
@@ -41439,7 +41439,7 @@
         <v>-0.251233841035465</v>
       </c>
       <c r="E2368" t="n">
-        <v>-0.251233841035465</v>
+        <v>-0.251196052246454</v>
       </c>
     </row>
     <row r="2369">
@@ -41456,7 +41456,7 @@
         <v>-0.360078268425278</v>
       </c>
       <c r="E2369" t="n">
-        <v>-0.451842919749402</v>
+        <v>-0.451843655379282</v>
       </c>
     </row>
     <row r="2370">
@@ -41473,7 +41473,7 @@
         <v>0.598964310364709</v>
       </c>
       <c r="E2370" t="n">
-        <v>0.596976590605983</v>
+        <v>0.596976294167106</v>
       </c>
     </row>
     <row r="2371">
@@ -41490,7 +41490,7 @@
         <v>0.53851277065279</v>
       </c>
       <c r="E2371" t="n">
-        <v>0.53712561556191</v>
+        <v>0.537125352883185</v>
       </c>
     </row>
     <row r="2372">
@@ -41507,7 +41507,7 @@
         <v>0.271307976738569</v>
       </c>
       <c r="E2372" t="n">
-        <v>0.270598266595251</v>
+        <v>0.270598004175779</v>
       </c>
     </row>
     <row r="2373">
@@ -41524,7 +41524,7 @@
         <v>0.387761129595832</v>
       </c>
       <c r="E2373" t="n">
-        <v>0.387110389591535</v>
+        <v>0.387110092511118</v>
       </c>
     </row>
     <row r="2374">
@@ -41541,7 +41541,7 @@
         <v>0.205856231790359</v>
       </c>
       <c r="E2374" t="n">
-        <v>0.205317079990256</v>
+        <v>0.205316780115145</v>
       </c>
     </row>
     <row r="2375">
@@ -41558,7 +41558,7 @@
         <v>0.15123515553915</v>
       </c>
       <c r="E2375" t="n">
-        <v>0.150873239869908</v>
+        <v>0.150872940358082</v>
       </c>
     </row>
     <row r="2376">
@@ -41575,7 +41575,7 @@
         <v>0.0926681834461529</v>
       </c>
       <c r="E2376" t="n">
-        <v>0.092497695746281</v>
+        <v>0.0924973942448058</v>
       </c>
     </row>
     <row r="2377">
@@ -41592,7 +41592,7 @@
         <v>0.0416487732744114</v>
       </c>
       <c r="E2377" t="n">
-        <v>0.0416421735808406</v>
+        <v>0.0416418771052817</v>
       </c>
     </row>
     <row r="2378">
@@ -42493,7 +42493,7 @@
         <v>180.474383266158</v>
       </c>
       <c r="E2430" t="n">
-        <v>187.753741471868</v>
+        <v>182.350621081697</v>
       </c>
     </row>
     <row r="2431">
@@ -42510,7 +42510,7 @@
         <v>180.474383266158</v>
       </c>
       <c r="E2431" t="n">
-        <v>187.933099677577</v>
+        <v>182.350621081697</v>
       </c>
     </row>
     <row r="2432">
@@ -42527,7 +42527,7 @@
         <v>180.474383266158</v>
       </c>
       <c r="E2432" t="n">
-        <v>187.958408770181</v>
+        <v>182.350621081697</v>
       </c>
     </row>
     <row r="2433">
@@ -42544,7 +42544,7 @@
         <v>180.474383266158</v>
       </c>
       <c r="E2433" t="n">
-        <v>187.983717862784</v>
+        <v>182.350621081697</v>
       </c>
     </row>
     <row r="2434">
@@ -42561,7 +42561,7 @@
         <v>222.122317866041</v>
       </c>
       <c r="E2434" t="n">
-        <v>229.656961555271</v>
+        <v>224.431533639012</v>
       </c>
     </row>
     <row r="2435">
@@ -42578,7 +42578,7 @@
         <v>222.12231786604</v>
       </c>
       <c r="E2435" t="n">
-        <v>229.682270647874</v>
+        <v>224.431533639012</v>
       </c>
     </row>
     <row r="2436">
@@ -42595,7 +42595,7 @@
         <v>222.122317866041</v>
       </c>
       <c r="E2436" t="n">
-        <v>229.600380937499</v>
+        <v>224.431533639011</v>
       </c>
     </row>
     <row r="2437">
@@ -42612,7 +42612,7 @@
         <v>219.689932353381</v>
       </c>
       <c r="E2437" t="n">
-        <v>227.086105714465</v>
+        <v>221.973860694428</v>
       </c>
     </row>
     <row r="2438">
@@ -42697,7 +42697,7 @@
         <v>0.0689893491314676</v>
       </c>
       <c r="E2442" t="n">
-        <v>0.0980448738116599</v>
+        <v>0.0760023174853236</v>
       </c>
     </row>
     <row r="2443">
@@ -42714,7 +42714,7 @@
         <v>-0.0980070782024959</v>
       </c>
       <c r="E2443" t="n">
-        <v>-0.0687225886142598</v>
+        <v>-0.0910492460376189</v>
       </c>
     </row>
     <row r="2444">
@@ -42731,7 +42731,7 @@
         <v>0.01267811703132</v>
       </c>
       <c r="E2444" t="n">
-        <v>0.041324539448548</v>
+        <v>0.0194110704866701</v>
       </c>
     </row>
     <row r="2445">
@@ -42748,7 +42748,7 @@
         <v>0.0383131211964224</v>
       </c>
       <c r="E2445" t="n">
-        <v>0.0388252964173525</v>
+        <v>0.0173151159857355</v>
       </c>
     </row>
     <row r="2446">
@@ -42765,7 +42765,7 @@
         <v>0.135204753436808</v>
       </c>
       <c r="E2446" t="n">
-        <v>0.135031266436354</v>
+        <v>0.136535433682856</v>
       </c>
     </row>
     <row r="2447">
@@ -42782,7 +42782,7 @@
         <v>0.132795597359758</v>
       </c>
       <c r="E2447" t="n">
-        <v>0.132041066742625</v>
+        <v>0.134102566779675</v>
       </c>
     </row>
     <row r="2448">
@@ -42799,7 +42799,7 @@
         <v>0.129433962696625</v>
       </c>
       <c r="E2448" t="n">
-        <v>0.128258836018957</v>
+        <v>0.130707847030944</v>
       </c>
     </row>
     <row r="2449">
@@ -42816,7 +42816,7 @@
         <v>0.117752355807007</v>
       </c>
       <c r="E2449" t="n">
-        <v>0.116203880950775</v>
+        <v>0.118911270192893</v>
       </c>
     </row>
     <row r="2450">
@@ -42901,7 +42901,7 @@
         <v>14.8879117768835</v>
       </c>
       <c r="E2454" t="n">
-        <v>15.0045708497111</v>
+        <v>9.6014504595411</v>
       </c>
     </row>
     <row r="2455">
@@ -42918,7 +42918,7 @@
         <v>-1.79086999540024</v>
       </c>
       <c r="E2455" t="n">
-        <v>-1.68374577636746</v>
+        <v>-1.80948813913525</v>
       </c>
     </row>
     <row r="2456">
@@ -42935,7 +42935,7 @@
         <v>-1.58616486132109</v>
       </c>
       <c r="E2456" t="n">
-        <v>-1.62640941499274</v>
+        <v>-1.60265486084748</v>
       </c>
     </row>
     <row r="2457">
@@ -42952,7 +42952,7 @@
         <v>-1.76324267858908</v>
       </c>
       <c r="E2457" t="n">
-        <v>-1.8110528450045</v>
+        <v>-1.78157360473804</v>
       </c>
     </row>
     <row r="2458">
@@ -42969,7 +42969,7 @@
         <v>39.9661315913177</v>
       </c>
       <c r="E2458" t="n">
-        <v>39.9214627663444</v>
+        <v>40.3816252811992</v>
       </c>
     </row>
     <row r="2459">
@@ -42986,7 +42986,7 @@
         <v>-2.06510435142249</v>
       </c>
       <c r="E2459" t="n">
-        <v>-2.10984596609836</v>
+        <v>-2.08657347522259</v>
       </c>
     </row>
     <row r="2460">
@@ -43003,7 +43003,7 @@
         <v>-2.09845541001079</v>
       </c>
       <c r="E2460" t="n">
-        <v>-2.25176623631313</v>
+        <v>-2.12027125624516</v>
       </c>
     </row>
     <row r="2461">
@@ -43020,7 +43020,7 @@
         <v>-4.51004156478197</v>
       </c>
       <c r="E2461" t="n">
-        <v>-4.66187851480282</v>
+        <v>-4.55692860980395</v>
       </c>
     </row>
     <row r="2462">
@@ -43105,7 +43105,7 @@
         <v>3.80284815016204</v>
       </c>
       <c r="E2466" t="n">
-        <v>5.40741990289757</v>
+        <v>4.19171781510931</v>
       </c>
     </row>
     <row r="2467">
@@ -43122,7 +43122,7 @@
         <v>-5.45775195643029</v>
       </c>
       <c r="E2467" t="n">
-        <v>-3.82907725441238</v>
+        <v>-5.07307137382339</v>
       </c>
     </row>
     <row r="2468">
@@ -43139,7 +43139,7 @@
         <v>0.716232021720566</v>
       </c>
       <c r="E2468" t="n">
-        <v>2.33585169916236</v>
+        <v>1.09720235443402</v>
       </c>
     </row>
     <row r="2469">
@@ -43156,7 +43156,7 @@
         <v>2.19321770435394</v>
       </c>
       <c r="E2469" t="n">
-        <v>2.22375663300295</v>
+        <v>0.991740117334572</v>
       </c>
     </row>
     <row r="2470">
@@ -43173,7 +43173,7 @@
         <v>7.83581716260165</v>
       </c>
       <c r="E2470" t="n">
-        <v>7.83005731424543</v>
+        <v>7.91727945220765</v>
       </c>
     </row>
     <row r="2471">
@@ -43190,7 +43190,7 @@
         <v>7.77411443249664</v>
       </c>
       <c r="E2471" t="n">
-        <v>7.73418477155598</v>
+        <v>7.854935251588</v>
       </c>
     </row>
     <row r="2472">
@@ -43207,7 +43207,7 @@
         <v>7.65884905904146</v>
       </c>
       <c r="E2472" t="n">
-        <v>7.59347948675889</v>
+        <v>7.73847156262352</v>
       </c>
     </row>
     <row r="2473">
@@ -43224,7 +43224,7 @@
         <v>7.04081930964806</v>
       </c>
       <c r="E2473" t="n">
-        <v>6.95204371105426</v>
+        <v>7.1140166864837</v>
       </c>
     </row>
     <row r="2474">
@@ -46165,7 +46165,7 @@
         <v>189.834446925</v>
       </c>
       <c r="E2646" t="n">
-        <v>189.82629591119</v>
+        <v>189.87565218125</v>
       </c>
     </row>
     <row r="2647">
@@ -46182,7 +46182,7 @@
         <v>190.563619159625</v>
       </c>
       <c r="E2647" t="n">
-        <v>190.517364388366</v>
+        <v>190.605030442156</v>
       </c>
     </row>
     <row r="2648">
@@ -46199,7 +46199,7 @@
         <v>191.662846303322</v>
       </c>
       <c r="E2648" t="n">
-        <v>191.708905493317</v>
+        <v>191.704568170472</v>
       </c>
     </row>
     <row r="2649">
@@ -46216,7 +46216,7 @@
         <v>193.139474766356</v>
       </c>
       <c r="E2649" t="n">
-        <v>193.279714393746</v>
+        <v>193.181613852178</v>
       </c>
     </row>
     <row r="2650">
@@ -46233,7 +46233,7 @@
         <v>206.479455749855</v>
       </c>
       <c r="E2650" t="n">
-        <v>206.715771908557</v>
+        <v>206.622153793172</v>
       </c>
     </row>
     <row r="2651">
@@ -46250,7 +46250,7 @@
         <v>218.84314335309</v>
       </c>
       <c r="E2651" t="n">
-        <v>219.16818028727</v>
+        <v>219.07867428159</v>
       </c>
     </row>
     <row r="2652">
@@ -46267,7 +46267,7 @@
         <v>241.911000037969</v>
       </c>
       <c r="E2652" t="n">
-        <v>242.424178290934</v>
+        <v>242.345290812083</v>
       </c>
     </row>
     <row r="2653">
@@ -46284,7 +46284,7 @@
         <v>263.893002880096</v>
       </c>
       <c r="E2653" t="n">
-        <v>264.58614122692</v>
+        <v>264.517460401194</v>
       </c>
     </row>
     <row r="2654">
@@ -46369,7 +46369,7 @@
         <v>0.163743091782177</v>
       </c>
       <c r="E2658" t="n">
-        <v>0.163323413488463</v>
+        <v>0.163524767203408</v>
       </c>
     </row>
     <row r="2659">
@@ -46386,7 +46386,7 @@
         <v>0.159553951647807</v>
       </c>
       <c r="E2659" t="n">
-        <v>0.158986374280743</v>
+        <v>0.159338409616885</v>
       </c>
     </row>
     <row r="2660">
@@ -46403,7 +46403,7 @@
         <v>0.158075142917114</v>
       </c>
       <c r="E2660" t="n">
-        <v>0.157884308232431</v>
+        <v>0.157862026687446</v>
       </c>
     </row>
     <row r="2661">
@@ -46420,7 +46420,7 @@
         <v>0.159263686292097</v>
       </c>
       <c r="E2661" t="n">
-        <v>0.159727390601749</v>
+        <v>0.159337233208956</v>
       </c>
     </row>
     <row r="2662">
@@ -46437,7 +46437,7 @@
         <v>0.0365482161765006</v>
       </c>
       <c r="E2662" t="n">
-        <v>0.0374718212625402</v>
+        <v>0.0369158764459904</v>
       </c>
     </row>
     <row r="2663">
@@ -46454,7 +46454,7 @@
         <v>0.0807599029567204</v>
       </c>
       <c r="E2663" t="n">
-        <v>0.0821282200230036</v>
+        <v>0.0814517090469519</v>
       </c>
     </row>
     <row r="2664">
@@ -46471,7 +46471,7 @@
         <v>0.161942518700986</v>
       </c>
       <c r="E2664" t="n">
-        <v>0.163602238105687</v>
+        <v>0.163329074561166</v>
       </c>
     </row>
     <row r="2665">
@@ -46488,7 +46488,7 @@
         <v>0.235951533179314</v>
       </c>
       <c r="E2665" t="n">
-        <v>0.237858730890504</v>
+        <v>0.237982042026701</v>
       </c>
     </row>
     <row r="2666">
@@ -46981,7 +46981,7 @@
         <v>42.6460238985939</v>
       </c>
       <c r="E2694" t="n">
-        <v>42.6378728847844</v>
+        <v>42.6872291548445</v>
       </c>
     </row>
     <row r="2695">
@@ -46998,7 +46998,7 @@
         <v>-1.1545788492609</v>
       </c>
       <c r="E2695" t="n">
-        <v>-1.19260172317561</v>
+        <v>-1.15478170791857</v>
       </c>
     </row>
     <row r="2696">
@@ -47015,7 +47015,7 @@
         <v>-0.575610642624639</v>
       </c>
       <c r="E2696" t="n">
-        <v>-0.48289015446349</v>
+        <v>-0.575664016147641</v>
       </c>
     </row>
     <row r="2697">
@@ -47032,7 +47032,7 @@
         <v>-0.395925992539304</v>
       </c>
       <c r="E2697" t="n">
-        <v>-0.302195555460258</v>
+        <v>-0.39591639834839</v>
       </c>
     </row>
     <row r="2698">
@@ -47049,7 +47049,7 @@
         <v>11.5401546377532</v>
       </c>
       <c r="E2698" t="n">
-        <v>11.6349243053264</v>
+        <v>11.6403209099259</v>
       </c>
     </row>
     <row r="2699">
@@ -47066,7 +47066,7 @@
         <v>10.4440172763412</v>
       </c>
       <c r="E2699" t="n">
-        <v>10.5305409852097</v>
+        <v>10.5355234765112</v>
       </c>
     </row>
     <row r="2700">
@@ -47083,7 +47083,7 @@
         <v>21.0003806089714</v>
       </c>
       <c r="E2700" t="n">
-        <v>21.1854512074464</v>
+        <v>21.1969153240545</v>
       </c>
     </row>
     <row r="2701">
@@ -47100,7 +47100,7 @@
         <v>19.7192502374701</v>
       </c>
       <c r="E2701" t="n">
-        <v>19.8944102377883</v>
+        <v>19.905354777361</v>
       </c>
     </row>
     <row r="2702">
@@ -47185,7 +47185,7 @@
         <v>9.02588764099011</v>
       </c>
       <c r="E2706" t="n">
-        <v>9.00769456242244</v>
+        <v>9.01879972318597</v>
       </c>
     </row>
     <row r="2707">
@@ -47202,7 +47202,7 @@
         <v>8.88513266320211</v>
       </c>
       <c r="E2707" t="n">
-        <v>8.85838443800363</v>
+        <v>8.87799910219999</v>
       </c>
     </row>
     <row r="2708">
@@ -47219,7 +47219,7 @@
         <v>8.93022827566562</v>
       </c>
       <c r="E2708" t="n">
-        <v>8.9243421603034</v>
+        <v>8.92308270562083</v>
       </c>
     </row>
     <row r="2709">
@@ -47236,7 +47236,7 @@
         <v>9.11697939318804</v>
       </c>
       <c r="E2709" t="n">
-        <v>9.14854172662913</v>
+        <v>9.12619508229672</v>
       </c>
     </row>
     <row r="2710">
@@ -47253,7 +47253,7 @@
         <v>2.11815880949888</v>
       </c>
       <c r="E2710" t="n">
-        <v>2.17287829625108</v>
+        <v>2.14064072719003</v>
       </c>
     </row>
     <row r="2711">
@@ -47270,7 +47270,7 @@
         <v>4.72784293775936</v>
       </c>
       <c r="E2711" t="n">
-        <v>4.81058540563777</v>
+        <v>4.77095939368674</v>
       </c>
     </row>
     <row r="2712">
@@ -47287,7 +47287,7 @@
         <v>9.58244096936847</v>
       </c>
       <c r="E2712" t="n">
-        <v>9.6859622120675</v>
+        <v>9.66978974523222</v>
       </c>
     </row>
     <row r="2713">
@@ -47304,7 +47304,7 @@
         <v>14.1083556211206</v>
       </c>
       <c r="E2713" t="n">
-        <v>14.2301985155484</v>
+        <v>14.2375757597668</v>
       </c>
     </row>
     <row r="2714">
@@ -47576,7 +47576,7 @@
         <v>0.00273134671266093</v>
       </c>
       <c r="E2729" t="n">
-        <v>0.00273090642075571</v>
+        <v>0.00170552334921903</v>
       </c>
     </row>
     <row r="2730">
@@ -47593,7 +47593,7 @@
         <v>0.00197811219324793</v>
       </c>
       <c r="E2730" t="n">
-        <v>0.00197670549752472</v>
+        <v>0.00142544110935494</v>
       </c>
     </row>
     <row r="2731">
@@ -47610,7 +47610,7 @@
         <v>0.00172558109055693</v>
       </c>
       <c r="E2731" t="n">
-        <v>0.00172435155408934</v>
+        <v>0.00132818541706793</v>
       </c>
     </row>
     <row r="2732">
@@ -47627,7 +47627,7 @@
         <v>0.00147706390088763</v>
       </c>
       <c r="E2732" t="n">
-        <v>0.00147600959240488</v>
+        <v>0.00123054492488808</v>
       </c>
     </row>
     <row r="2733">
@@ -47644,7 +47644,7 @@
         <v>0.00123247354412561</v>
       </c>
       <c r="E2733" t="n">
-        <v>0.00123159101540816</v>
+        <v>0.00113382258094665</v>
       </c>
     </row>
     <row r="2734">
@@ -47661,7 +47661,7 @@
         <v>0.00121358552334201</v>
       </c>
       <c r="E2734" t="n">
-        <v>0.00121271588688309</v>
+        <v>0.00111676563874279</v>
       </c>
     </row>
     <row r="2735">
@@ -47678,7 +47678,7 @@
         <v>0.00119718033635228</v>
       </c>
       <c r="E2735" t="n">
-        <v>0.00119632174260091</v>
+        <v>0.00110153541568222</v>
       </c>
     </row>
     <row r="2736">
@@ -47695,7 +47695,7 @@
         <v>0.00117911066499121</v>
       </c>
       <c r="E2736" t="n">
-        <v>0.00117826413207413</v>
+        <v>0.00108525955044049</v>
       </c>
     </row>
     <row r="2737">
@@ -47712,7 +47712,7 @@
         <v>0.000953682373449863</v>
       </c>
       <c r="E2737" t="n">
-        <v>0.000952994516782712</v>
+        <v>0.000998128807608058</v>
       </c>
     </row>
     <row r="2738">
@@ -48392,7 +48392,7 @@
         <v>0.146773695461582</v>
       </c>
       <c r="E2777" t="n">
-        <v>0.146750035605545</v>
+        <v>0.0916492818361457</v>
       </c>
     </row>
     <row r="2778">
@@ -48409,7 +48409,7 @@
         <v>0.10903799484426</v>
       </c>
       <c r="E2778" t="n">
-        <v>0.109020249952232</v>
+        <v>0.0786166407836986</v>
       </c>
     </row>
     <row r="2779">
@@ -48426,7 +48426,7 @@
         <v>0.0960929939520058</v>
       </c>
       <c r="E2779" t="n">
-        <v>0.0960772207146472</v>
+        <v>0.0740036816523782</v>
       </c>
     </row>
     <row r="2780">
@@ -48443,7 +48443,7 @@
         <v>0.0834446046940353</v>
       </c>
       <c r="E2780" t="n">
-        <v>0.0834308031113465</v>
+        <v>0.0695560190640292</v>
       </c>
     </row>
     <row r="2781">
@@ -48460,7 +48460,7 @@
         <v>0.0705524037904942</v>
       </c>
       <c r="E2781" t="n">
-        <v>0.0705405738624752</v>
+        <v>0.0649407916407244</v>
       </c>
     </row>
     <row r="2782">
@@ -48477,7 +48477,7 @@
         <v>0.0703335794812328</v>
       </c>
       <c r="E2782" t="n">
-        <v>0.0703217495532138</v>
+        <v>0.0647578830348712</v>
       </c>
     </row>
     <row r="2783">
@@ -48494,7 +48494,7 @@
         <v>0.0700852823149226</v>
       </c>
       <c r="E2783" t="n">
-        <v>0.0700734523869036</v>
+        <v>0.0645214299419834</v>
       </c>
     </row>
     <row r="2784">
@@ -48511,7 +48511,7 @@
         <v>0.0697701779264856</v>
       </c>
       <c r="E2784" t="n">
-        <v>0.0697583479984667</v>
+        <v>0.0642520733063646</v>
       </c>
     </row>
     <row r="2785">
@@ -48528,7 +48528,7 @@
         <v>0.0570239569666191</v>
       </c>
       <c r="E2785" t="n">
-        <v>0.05701409869327</v>
+        <v>0.0597143145562682</v>
       </c>
     </row>
     <row r="2786">
@@ -48800,7 +48800,7 @@
         <v>-0.423001925559832</v>
       </c>
       <c r="E2801" t="n">
-        <v>-0.417735269886195</v>
+        <v>-0.418760652957732</v>
       </c>
     </row>
     <row r="2802">
@@ -48817,7 +48817,7 @@
         <v>-0.092144918521197</v>
       </c>
       <c r="E2802" t="n">
-        <v>-0.0765545099540014</v>
+        <v>-0.0989469769535621</v>
       </c>
     </row>
     <row r="2803">
@@ -48834,7 +48834,7 @@
         <v>-0.186973919601332</v>
       </c>
       <c r="E2803" t="n">
-        <v>-0.157860116866743</v>
+        <v>-0.180230905090981</v>
       </c>
     </row>
     <row r="2804">
@@ -48851,7 +48851,7 @@
         <v>-0.160402774443666</v>
       </c>
       <c r="E2804" t="n">
-        <v>-0.138527540883996</v>
+        <v>-0.160708756058376</v>
       </c>
     </row>
     <row r="2805">
@@ -48868,7 +48868,7 @@
         <v>0.0283198711427655</v>
       </c>
       <c r="E2805" t="n">
-        <v>0.024094131496119</v>
+        <v>0.00209602523724745</v>
       </c>
     </row>
     <row r="2806">
@@ -48885,7 +48885,7 @@
         <v>-0.0168568321961238</v>
       </c>
       <c r="E2806" t="n">
-        <v>-0.0225695864319424</v>
+        <v>-0.02171731425013</v>
       </c>
     </row>
     <row r="2807">
@@ -48902,7 +48902,7 @@
         <v>0.0889387571443329</v>
       </c>
       <c r="E2807" t="n">
-        <v>0.0844727750266013</v>
+        <v>0.0857629777606806</v>
       </c>
     </row>
     <row r="2808">
@@ -48919,7 +48919,7 @@
         <v>0.207721651248892</v>
       </c>
       <c r="E2808" t="n">
-        <v>0.201819453134494</v>
+        <v>0.203902296020327</v>
       </c>
     </row>
     <row r="2809">
@@ -48936,7 +48936,7 @@
         <v>0.0623066017818567</v>
       </c>
       <c r="E2809" t="n">
-        <v>0.0623287213688381</v>
+        <v>0.0652045560379787</v>
       </c>
     </row>
     <row r="2810">
@@ -49208,7 +49208,7 @@
         <v>-0.318389943826779</v>
       </c>
       <c r="E2825" t="n">
-        <v>-0.299666243968138</v>
+        <v>-0.300691627039675</v>
       </c>
     </row>
     <row r="2826">
@@ -49225,7 +49225,7 @@
         <v>-0.047621103079969</v>
       </c>
       <c r="E2826" t="n">
-        <v>-0.0189218927700582</v>
+        <v>-0.0413143597696189</v>
       </c>
     </row>
     <row r="2827">
@@ -49242,7 +49242,7 @@
         <v>-0.111636633820175</v>
       </c>
       <c r="E2827" t="n">
-        <v>-0.0757891338741147</v>
+        <v>-0.0981599220983525</v>
       </c>
     </row>
     <row r="2828">
@@ -49259,7 +49259,7 @@
         <v>-0.053787015376182</v>
       </c>
       <c r="E2828" t="n">
-        <v>-0.0252336292195443</v>
+        <v>-0.0474148443939242</v>
       </c>
     </row>
     <row r="2829">
@@ -49276,7 +49276,7 @@
         <v>0.1164287187215</v>
       </c>
       <c r="E2829" t="n">
-        <v>0.118810361635989</v>
+        <v>0.0968122553771177</v>
       </c>
     </row>
     <row r="2830">
@@ -49293,7 +49293,7 @@
         <v>0.1512158025131</v>
       </c>
       <c r="E2830" t="n">
-        <v>0.15196474093267</v>
+        <v>0.152817013114483</v>
       </c>
     </row>
     <row r="2831">
@@ -49310,7 +49310,7 @@
         <v>0.186594231255333</v>
       </c>
       <c r="E2831" t="n">
-        <v>0.188566009931411</v>
+        <v>0.189856212665491</v>
       </c>
     </row>
     <row r="2832">
@@ -49327,7 +49327,7 @@
         <v>0.285993456356236</v>
       </c>
       <c r="E2832" t="n">
-        <v>0.286480801745404</v>
+        <v>0.288563644631237</v>
       </c>
     </row>
     <row r="2833">
@@ -49344,7 +49344,7 @@
         <v>0.116583888737229</v>
       </c>
       <c r="E2833" t="n">
-        <v>0.117072502202486</v>
+        <v>0.119948336871626</v>
       </c>
     </row>
     <row r="2834">
@@ -51452,7 +51452,7 @@
         <v>0.509039692443663</v>
       </c>
       <c r="E2957" t="n">
-        <v>0.508591768812085</v>
+        <v>0.450594397425785</v>
       </c>
     </row>
     <row r="2958">
@@ -51469,7 +51469,7 @@
         <v>-0.700472647159408</v>
       </c>
       <c r="E2958" t="n">
-        <v>-0.700415771633917</v>
+        <v>-0.281545262775178</v>
       </c>
     </row>
     <row r="2959">
@@ -51486,7 +51486,7 @@
         <v>-0.383234531480189</v>
       </c>
       <c r="E2959" t="n">
-        <v>-0.383312333319647</v>
+        <v>-0.17224418140345</v>
       </c>
     </row>
     <row r="2960">
@@ -51503,7 +51503,7 @@
         <v>-0.246020824565572</v>
       </c>
       <c r="E2960" t="n">
-        <v>-0.24613428916138</v>
+        <v>-0.133035661640124</v>
       </c>
     </row>
     <row r="2961">
@@ -51520,7 +51520,7 @@
         <v>-0.165381732204281</v>
       </c>
       <c r="E2961" t="n">
-        <v>-0.165501146426298</v>
+        <v>-0.101337592086262</v>
       </c>
     </row>
     <row r="2962">
@@ -51537,7 +51537,7 @@
         <v>-0.185347236498705</v>
       </c>
       <c r="E2962" t="n">
-        <v>-0.185453123586975</v>
+        <v>-0.103366630904651</v>
       </c>
     </row>
     <row r="2963">
@@ -51554,7 +51554,7 @@
         <v>-0.207517806273682</v>
       </c>
       <c r="E2963" t="n">
-        <v>-0.207609453018507</v>
+        <v>-0.118397835651029</v>
       </c>
     </row>
     <row r="2964">
@@ -51571,7 +51571,7 @@
         <v>-0.136441943855362</v>
       </c>
       <c r="E2964" t="n">
-        <v>-0.136570386971856</v>
+        <v>-0.0929314277531034</v>
       </c>
     </row>
     <row r="2965">
@@ -51588,7 +51588,7 @@
         <v>-0.146419030233699</v>
       </c>
       <c r="E2965" t="n">
-        <v>-0.146506360360885</v>
+        <v>-0.0933633731719349</v>
       </c>
     </row>
     <row r="2966">
@@ -52064,7 +52064,7 @@
         <v>27.354138692922</v>
       </c>
       <c r="E2993" t="n">
-        <v>27.3300687327128</v>
+        <v>24.21347848587</v>
       </c>
     </row>
     <row r="2994">
@@ -52081,7 +52081,7 @@
         <v>-38.6116283748827</v>
       </c>
       <c r="E2994" t="n">
-        <v>-38.6296808450396</v>
+        <v>-15.527925105208</v>
       </c>
     </row>
     <row r="2995">
@@ -52098,7 +52098,7 @@
         <v>-21.3413056721895</v>
       </c>
       <c r="E2995" t="n">
-        <v>-21.357352312329</v>
+        <v>-9.59708140388612</v>
       </c>
     </row>
     <row r="2996">
@@ -52115,7 +52115,7 @@
         <v>-13.8985933107145</v>
       </c>
       <c r="E2996" t="n">
-        <v>-13.9126341208366</v>
+        <v>-7.51978317092147</v>
       </c>
     </row>
     <row r="2997">
@@ -52132,7 +52132,7 @@
         <v>-9.46720422978803</v>
       </c>
       <c r="E2997" t="n">
-        <v>-9.47923920989265</v>
+        <v>-5.80420919783773</v>
       </c>
     </row>
     <row r="2998">
@@ -52149,7 +52149,7 @@
         <v>-10.7418342911748</v>
       </c>
       <c r="E2998" t="n">
-        <v>-10.7538692712794</v>
+        <v>-5.99392026546206</v>
       </c>
     </row>
     <row r="2999">
@@ -52166,7 +52166,7 @@
         <v>-12.1484989323987</v>
       </c>
       <c r="E2999" t="n">
-        <v>-12.1605339125033</v>
+        <v>-6.93504498310577</v>
       </c>
     </row>
     <row r="3000">
@@ -52183,7 +52183,7 @@
         <v>-8.07352437906681</v>
       </c>
       <c r="E3000" t="n">
-        <v>-8.08555935917142</v>
+        <v>-5.50194366502832</v>
       </c>
     </row>
     <row r="3001">
@@ -52200,7 +52200,7 @@
         <v>-8.7548986031244</v>
       </c>
       <c r="E3001" t="n">
-        <v>-8.76492775321158</v>
+        <v>-5.58558153128909</v>
       </c>
     </row>
     <row r="3002">
@@ -52472,7 +52472,7 @@
         <v>8.50292322474818</v>
       </c>
       <c r="E3017" t="n">
-        <v>8.35156014777995</v>
+        <v>6.78844756194544</v>
       </c>
     </row>
     <row r="3018">
@@ -52489,7 +52489,7 @@
         <v>-1.2038193555033</v>
       </c>
       <c r="E3018" t="n">
-        <v>-1.29414674011778</v>
+        <v>0.772080685801949</v>
       </c>
     </row>
     <row r="3019">
@@ -52506,7 +52506,7 @@
         <v>-2.56091357421352</v>
       </c>
       <c r="E3019" t="n">
-        <v>-2.62791220636268</v>
+        <v>-2.36702653173626</v>
       </c>
     </row>
     <row r="3020">
@@ -52523,7 +52523,7 @@
         <v>-2.06996720849503</v>
       </c>
       <c r="E3020" t="n">
-        <v>-2.14051987123165</v>
+        <v>-2.0882458152339</v>
       </c>
     </row>
     <row r="3021">
@@ -52540,7 +52540,7 @@
         <v>-0.870359602854143</v>
       </c>
       <c r="E3021" t="n">
-        <v>-0.951009621947622</v>
+        <v>-0.85659864946568</v>
       </c>
     </row>
     <row r="3022">
@@ -52557,7 +52557,7 @@
         <v>-4.06662679934688</v>
       </c>
       <c r="E3022" t="n">
-        <v>-4.14820231508265</v>
+        <v>-3.9772713199995</v>
       </c>
     </row>
     <row r="3023">
@@ -52574,7 +52574,7 @@
         <v>-2.5864234111831</v>
       </c>
       <c r="E3023" t="n">
-        <v>-2.67092268403431</v>
+        <v>-2.42927071948584</v>
       </c>
     </row>
     <row r="3024">
@@ -52591,7 +52591,7 @@
         <v>-0.770282826774579</v>
       </c>
       <c r="E3024" t="n">
-        <v>-0.804890272618345</v>
+        <v>-0.715151997146874</v>
       </c>
     </row>
     <row r="3025">
@@ -52608,7 +52608,7 @@
         <v>-1.70506905052958</v>
       </c>
       <c r="E3025" t="n">
-        <v>-1.72053448881388</v>
+        <v>-1.57569612059391</v>
       </c>
     </row>
     <row r="3026">
@@ -52676,7 +52676,7 @@
         <v>8.51247725147007</v>
       </c>
       <c r="E3029" t="n">
-        <v>8.51799485451027</v>
+        <v>6.95488226867576</v>
       </c>
     </row>
     <row r="3030">
@@ -52693,7 +52693,7 @@
         <v>-1.27233404255178</v>
       </c>
       <c r="E3030" t="n">
-        <v>-1.26332350605143</v>
+        <v>0.8029039198683</v>
       </c>
     </row>
     <row r="3031">
@@ -52710,7 +52710,7 @@
         <v>-2.61162425955222</v>
       </c>
       <c r="E3031" t="n">
-        <v>-2.59984608559174</v>
+        <v>-2.33896041096532</v>
       </c>
     </row>
     <row r="3032">
@@ -52727,7 +52727,7 @@
         <v>-1.95437688813453</v>
       </c>
       <c r="E3032" t="n">
-        <v>-1.94342106141575</v>
+        <v>-1.891147005418</v>
       </c>
     </row>
     <row r="3033">
@@ -52744,7 +52744,7 @@
         <v>-0.61975241451693</v>
       </c>
       <c r="E3033" t="n">
-        <v>-0.616303513197983</v>
+        <v>-0.521892540716041</v>
       </c>
     </row>
     <row r="3034">
@@ -52761,7 +52761,7 @@
         <v>-3.38015629708815</v>
       </c>
       <c r="E3034" t="n">
-        <v>-3.37675302072768</v>
+        <v>-3.20582202564452</v>
       </c>
     </row>
     <row r="3035">
@@ -52778,7 +52778,7 @@
         <v>-1.99154710401809</v>
       </c>
       <c r="E3035" t="n">
-        <v>-1.98967860751212</v>
+        <v>-1.74802664296365</v>
       </c>
     </row>
     <row r="3036">
@@ -52795,7 +52795,7 @@
         <v>-0.297148752897317</v>
       </c>
       <c r="E3036" t="n">
-        <v>-0.29634710968282</v>
+        <v>-0.206608834211348</v>
       </c>
     </row>
     <row r="3037">
@@ -52812,7 +52812,7 @@
         <v>-1.28129365850713</v>
       </c>
       <c r="E3037" t="n">
-        <v>-1.28000529032886</v>
+        <v>-1.13516692210889</v>
       </c>
     </row>
     <row r="3038">

</xml_diff>